<commit_message>
data.py is now finished
</commit_message>
<xml_diff>
--- a/HiggsData.xlsx
+++ b/HiggsData.xlsx
@@ -4,8 +4,8 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Branching Ratios" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="7och8 TeV" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="13 Tev" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="7 and 8 TeV" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="13 TeV" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -192,7 +192,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="65">
   <si>
     <t>Process</t>
   </si>
@@ -225,6 +225,12 @@
     <t>5.792E-01</t>
   </si>
   <si>
+    <t>H -&gt; cc</t>
+  </si>
+  <si>
+    <t>2.876E-02</t>
+  </si>
+  <si>
     <t>H -&gt; tau tau</t>
   </si>
   <si>
@@ -237,28 +243,16 @@
     <t>2.165E-04</t>
   </si>
   <si>
-    <t>H -&gt; cc</t>
+    <t>H -&gt; gamma gamma</t>
   </si>
   <si>
-    <t>2.876E-02</t>
+    <t>2.270E-03</t>
   </si>
   <si>
     <t>H -&gt; gg</t>
   </si>
   <si>
     <t>8.172E-02</t>
-  </si>
-  <si>
-    <t>H -&gt; gamma gamma</t>
-  </si>
-  <si>
-    <t>2.270E-03</t>
-  </si>
-  <si>
-    <t>H -&gt; Z gamma</t>
-  </si>
-  <si>
-    <t>1.550E-03</t>
   </si>
   <si>
     <t>H -&gt; WW</t>
@@ -273,10 +267,16 @@
     <t>2.667E-02</t>
   </si>
   <si>
+    <t>H -&gt; Z gamma</t>
+  </si>
+  <si>
+    <t>1.550E-03</t>
+  </si>
+  <si>
     <t>avg, atlas</t>
   </si>
   <si>
-    <t>ggH</t>
+    <t>ggF</t>
   </si>
   <si>
     <t>VBF</t>
@@ -301,9 +301,6 @@
   </si>
   <si>
     <t>mu mu</t>
-  </si>
-  <si>
-    <t>no data</t>
   </si>
   <si>
     <t>https://arxiv.org/pdf/1406.7663.pdf</t>
@@ -372,9 +369,6 @@
     <t>https://arxiv.org/pdf/2004.03447.pdf</t>
   </si>
   <si>
-    <t>finns ingen vettig data på detta</t>
-  </si>
-  <si>
     <t>https://arxiv.org/pdf/2005.05382.pdf</t>
   </si>
   <si>
@@ -421,9 +415,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0000000"/>
-    <numFmt numFmtId="165" formatCode="hh.mm"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -466,7 +459,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -492,9 +485,6 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="4" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -756,7 +746,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="3">
-        <v>0.0624</v>
+        <v>0.02876</v>
       </c>
     </row>
     <row r="4">
@@ -767,7 +757,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="3">
-        <v>2.165E-4</v>
+        <v>0.0624</v>
       </c>
     </row>
     <row r="5">
@@ -778,7 +768,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="3">
-        <v>0.02876</v>
+        <v>2.165E-4</v>
       </c>
     </row>
     <row r="6">
@@ -789,7 +779,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="3">
-        <v>0.08172</v>
+        <v>0.00227</v>
       </c>
     </row>
     <row r="7">
@@ -800,7 +790,7 @@
         <v>16</v>
       </c>
       <c r="C7" s="3">
-        <v>0.00227</v>
+        <v>0.08172</v>
       </c>
     </row>
     <row r="8">
@@ -811,7 +801,7 @@
         <v>18</v>
       </c>
       <c r="C8" s="3">
-        <v>0.00155</v>
+        <v>0.217</v>
       </c>
     </row>
     <row r="9">
@@ -822,7 +812,7 @@
         <v>20</v>
       </c>
       <c r="C9" s="3">
-        <v>0.217</v>
+        <v>0.02667</v>
       </c>
     </row>
     <row r="10">
@@ -833,14 +823,14 @@
         <v>22</v>
       </c>
       <c r="C10" s="3">
-        <v>0.02667</v>
+        <v>0.00155</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="6"/>
       <c r="C11" s="7">
-        <f>SUM(C2:C10)</f>
-        <v>0.9997865</v>
+        <f>SUM(C2:C9)</f>
+        <v>0.9982365</v>
       </c>
     </row>
     <row r="12">
@@ -4878,16 +4868,13 @@
       <c r="A5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="F5" s="9" t="s">
         <v>33</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" s="1">
         <v>1.32</v>
@@ -4902,17 +4889,17 @@
         <v>1.6</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" s="1">
         <v>0.98</v>
@@ -4927,12 +4914,12 @@
         <v>2.1</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B9" s="1">
         <v>1.66</v>
@@ -4944,17 +4931,17 @@
         <v>2.1</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>24</v>
@@ -5014,7 +5001,7 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B18" s="1">
         <v>0.38</v>
@@ -5031,12 +5018,12 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20" s="1">
         <v>0.29</v>
@@ -5053,7 +5040,7 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B21" s="10">
         <f>0.45+0.25</f>
@@ -5069,12 +5056,12 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>24</v>
@@ -5122,7 +5109,7 @@
         <v>-1.3</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29">
@@ -5130,12 +5117,12 @@
         <v>32</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B30" s="1">
         <v>1.12</v>
@@ -5150,17 +5137,17 @@
         <v>2.69</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C32" s="1">
         <v>0.6</v>
@@ -5169,12 +5156,12 @@
         <v>0.39</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B33" s="1">
         <v>0.8</v>
@@ -5189,17 +5176,17 @@
         <v>0.8</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>24</v>
@@ -5254,7 +5241,7 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B42" s="1">
         <v>0.37</v>
@@ -5271,12 +5258,12 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C44" s="1">
         <v>0.57</v>
@@ -5287,7 +5274,7 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B45" s="1">
         <v>0.46</v>
@@ -5304,7 +5291,7 @@
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -5352,7 +5339,7 @@
         <v>27</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2">
@@ -5369,7 +5356,7 @@
         <v>0.79</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3">
@@ -5397,7 +5384,7 @@
         <v>1.06</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5">
@@ -5410,7 +5397,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" s="1">
         <v>1.04</v>
@@ -5425,17 +5412,17 @@
         <v>0.89</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" s="1">
         <v>1.1</v>
@@ -5446,19 +5433,16 @@
       <c r="D8" s="1">
         <v>0.92</v>
       </c>
-      <c r="F8" s="9" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B9" s="1">
         <v>0.96</v>
       </c>
-      <c r="C9" s="11">
-        <v>0.05625</v>
+      <c r="C9" s="1">
+        <v>1.21</v>
       </c>
       <c r="D9" s="1">
         <v>1.44</v>
@@ -5466,21 +5450,21 @@
       <c r="E9" s="1">
         <v>1.7</v>
       </c>
+      <c r="F9" s="9" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>57</v>
+        <v>41</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>24</v>
@@ -5544,7 +5528,7 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B18" s="1">
         <v>0.1</v>
@@ -5561,12 +5545,12 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20" s="1">
         <v>0.21</v>
@@ -5580,7 +5564,7 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B21" s="10">
         <f>0.1+0.03+0.03</f>
@@ -5599,17 +5583,17 @@
         <v>2.1</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>24</v>
@@ -5649,7 +5633,7 @@
         <v>2.4</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28">
@@ -5666,7 +5650,7 @@
         <v>0.28</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29">
@@ -5686,12 +5670,12 @@
         <v>2.32</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B30" s="1">
         <v>1.1</v>
@@ -5706,20 +5690,20 @@
         <v>2.2</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B32" s="1">
         <v>0.92</v>
@@ -5731,15 +5715,15 @@
         <v>1.97</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B33" s="1">
         <v>1.2</v>
@@ -5754,20 +5738,17 @@
         <v>0.0</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>24</v>
@@ -5844,7 +5825,7 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B42" s="1">
         <v>0.2</v>
@@ -5861,12 +5842,12 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B44" s="1">
         <v>0.11</v>
@@ -5880,7 +5861,7 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B45" s="1">
         <v>0.22</v>
@@ -5897,2870 +5878,2870 @@
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="47">
-      <c r="C47" s="12"/>
+      <c r="C47" s="11"/>
     </row>
     <row r="48">
-      <c r="C48" s="12"/>
+      <c r="C48" s="11"/>
     </row>
     <row r="49">
-      <c r="C49" s="12"/>
+      <c r="C49" s="11"/>
     </row>
     <row r="50">
-      <c r="C50" s="12"/>
+      <c r="C50" s="11"/>
     </row>
     <row r="51">
-      <c r="C51" s="12"/>
+      <c r="C51" s="11"/>
     </row>
     <row r="52">
-      <c r="C52" s="12"/>
+      <c r="C52" s="11"/>
     </row>
     <row r="53">
-      <c r="C53" s="12"/>
+      <c r="C53" s="11"/>
     </row>
     <row r="54">
-      <c r="C54" s="12"/>
+      <c r="C54" s="11"/>
     </row>
     <row r="55">
-      <c r="C55" s="12"/>
+      <c r="C55" s="11"/>
     </row>
     <row r="56">
-      <c r="C56" s="12"/>
+      <c r="C56" s="11"/>
     </row>
     <row r="57">
-      <c r="C57" s="12"/>
+      <c r="C57" s="11"/>
     </row>
     <row r="58">
-      <c r="C58" s="12"/>
+      <c r="C58" s="11"/>
     </row>
     <row r="59">
-      <c r="C59" s="12"/>
+      <c r="C59" s="11"/>
     </row>
     <row r="60">
-      <c r="C60" s="12"/>
+      <c r="C60" s="11"/>
     </row>
     <row r="61">
-      <c r="C61" s="12"/>
+      <c r="C61" s="11"/>
     </row>
     <row r="62">
-      <c r="C62" s="12"/>
+      <c r="C62" s="11"/>
     </row>
     <row r="63">
-      <c r="C63" s="12"/>
+      <c r="C63" s="11"/>
     </row>
     <row r="64">
-      <c r="C64" s="12"/>
+      <c r="C64" s="11"/>
     </row>
     <row r="65">
-      <c r="C65" s="12"/>
+      <c r="C65" s="11"/>
     </row>
     <row r="66">
-      <c r="C66" s="12"/>
+      <c r="C66" s="11"/>
     </row>
     <row r="67">
-      <c r="C67" s="12"/>
+      <c r="C67" s="11"/>
     </row>
     <row r="68">
-      <c r="C68" s="12"/>
+      <c r="C68" s="11"/>
     </row>
     <row r="69">
-      <c r="C69" s="12"/>
+      <c r="C69" s="11"/>
     </row>
     <row r="70">
-      <c r="C70" s="12"/>
+      <c r="C70" s="11"/>
     </row>
     <row r="71">
-      <c r="C71" s="12"/>
+      <c r="C71" s="11"/>
     </row>
     <row r="72">
-      <c r="C72" s="12"/>
+      <c r="C72" s="11"/>
     </row>
     <row r="73">
-      <c r="C73" s="12"/>
+      <c r="C73" s="11"/>
     </row>
     <row r="74">
-      <c r="C74" s="12"/>
+      <c r="C74" s="11"/>
     </row>
     <row r="75">
-      <c r="C75" s="12"/>
+      <c r="C75" s="11"/>
     </row>
     <row r="76">
-      <c r="C76" s="12"/>
+      <c r="C76" s="11"/>
     </row>
     <row r="77">
-      <c r="C77" s="12"/>
+      <c r="C77" s="11"/>
     </row>
     <row r="78">
-      <c r="C78" s="12"/>
+      <c r="C78" s="11"/>
     </row>
     <row r="79">
-      <c r="C79" s="12"/>
+      <c r="C79" s="11"/>
     </row>
     <row r="80">
-      <c r="C80" s="12"/>
+      <c r="C80" s="11"/>
     </row>
     <row r="81">
-      <c r="C81" s="12"/>
+      <c r="C81" s="11"/>
     </row>
     <row r="82">
-      <c r="C82" s="12"/>
+      <c r="C82" s="11"/>
     </row>
     <row r="83">
-      <c r="C83" s="12"/>
+      <c r="C83" s="11"/>
     </row>
     <row r="84">
-      <c r="C84" s="12"/>
+      <c r="C84" s="11"/>
     </row>
     <row r="85">
-      <c r="C85" s="12"/>
+      <c r="C85" s="11"/>
     </row>
     <row r="86">
-      <c r="C86" s="12"/>
+      <c r="C86" s="11"/>
     </row>
     <row r="87">
-      <c r="C87" s="12"/>
+      <c r="C87" s="11"/>
     </row>
     <row r="88">
-      <c r="C88" s="12"/>
+      <c r="C88" s="11"/>
     </row>
     <row r="89">
-      <c r="C89" s="12"/>
+      <c r="C89" s="11"/>
     </row>
     <row r="90">
-      <c r="C90" s="12"/>
+      <c r="C90" s="11"/>
     </row>
     <row r="91">
-      <c r="C91" s="12"/>
+      <c r="C91" s="11"/>
     </row>
     <row r="92">
-      <c r="C92" s="12"/>
+      <c r="C92" s="11"/>
     </row>
     <row r="93">
-      <c r="C93" s="12"/>
+      <c r="C93" s="11"/>
     </row>
     <row r="94">
-      <c r="C94" s="12"/>
+      <c r="C94" s="11"/>
     </row>
     <row r="95">
-      <c r="C95" s="12"/>
+      <c r="C95" s="11"/>
     </row>
     <row r="96">
-      <c r="C96" s="12"/>
+      <c r="C96" s="11"/>
     </row>
     <row r="97">
-      <c r="C97" s="12"/>
+      <c r="C97" s="11"/>
     </row>
     <row r="98">
-      <c r="C98" s="12"/>
+      <c r="C98" s="11"/>
     </row>
     <row r="99">
-      <c r="C99" s="12"/>
+      <c r="C99" s="11"/>
     </row>
     <row r="100">
-      <c r="C100" s="12"/>
+      <c r="C100" s="11"/>
     </row>
     <row r="101">
-      <c r="C101" s="12"/>
+      <c r="C101" s="11"/>
     </row>
     <row r="102">
-      <c r="C102" s="12"/>
+      <c r="C102" s="11"/>
     </row>
     <row r="103">
-      <c r="C103" s="12"/>
+      <c r="C103" s="11"/>
     </row>
     <row r="104">
-      <c r="C104" s="12"/>
+      <c r="C104" s="11"/>
     </row>
     <row r="105">
-      <c r="C105" s="12"/>
+      <c r="C105" s="11"/>
     </row>
     <row r="106">
-      <c r="C106" s="12"/>
+      <c r="C106" s="11"/>
     </row>
     <row r="107">
-      <c r="C107" s="12"/>
+      <c r="C107" s="11"/>
     </row>
     <row r="108">
-      <c r="C108" s="12"/>
+      <c r="C108" s="11"/>
     </row>
     <row r="109">
-      <c r="C109" s="12"/>
+      <c r="C109" s="11"/>
     </row>
     <row r="110">
-      <c r="C110" s="12"/>
+      <c r="C110" s="11"/>
     </row>
     <row r="111">
-      <c r="C111" s="12"/>
+      <c r="C111" s="11"/>
     </row>
     <row r="112">
-      <c r="C112" s="12"/>
+      <c r="C112" s="11"/>
     </row>
     <row r="113">
-      <c r="C113" s="12"/>
+      <c r="C113" s="11"/>
     </row>
     <row r="114">
-      <c r="C114" s="12"/>
+      <c r="C114" s="11"/>
     </row>
     <row r="115">
-      <c r="C115" s="12"/>
+      <c r="C115" s="11"/>
     </row>
     <row r="116">
-      <c r="C116" s="12"/>
+      <c r="C116" s="11"/>
     </row>
     <row r="117">
-      <c r="C117" s="12"/>
+      <c r="C117" s="11"/>
     </row>
     <row r="118">
-      <c r="C118" s="12"/>
+      <c r="C118" s="11"/>
     </row>
     <row r="119">
-      <c r="C119" s="12"/>
+      <c r="C119" s="11"/>
     </row>
     <row r="120">
-      <c r="C120" s="12"/>
+      <c r="C120" s="11"/>
     </row>
     <row r="121">
-      <c r="C121" s="12"/>
+      <c r="C121" s="11"/>
     </row>
     <row r="122">
-      <c r="C122" s="12"/>
+      <c r="C122" s="11"/>
     </row>
     <row r="123">
-      <c r="C123" s="12"/>
+      <c r="C123" s="11"/>
     </row>
     <row r="124">
-      <c r="C124" s="12"/>
+      <c r="C124" s="11"/>
     </row>
     <row r="125">
-      <c r="C125" s="12"/>
+      <c r="C125" s="11"/>
     </row>
     <row r="126">
-      <c r="C126" s="12"/>
+      <c r="C126" s="11"/>
     </row>
     <row r="127">
-      <c r="C127" s="12"/>
+      <c r="C127" s="11"/>
     </row>
     <row r="128">
-      <c r="C128" s="12"/>
+      <c r="C128" s="11"/>
     </row>
     <row r="129">
-      <c r="C129" s="12"/>
+      <c r="C129" s="11"/>
     </row>
     <row r="130">
-      <c r="C130" s="12"/>
+      <c r="C130" s="11"/>
     </row>
     <row r="131">
-      <c r="C131" s="12"/>
+      <c r="C131" s="11"/>
     </row>
     <row r="132">
-      <c r="C132" s="12"/>
+      <c r="C132" s="11"/>
     </row>
     <row r="133">
-      <c r="C133" s="12"/>
+      <c r="C133" s="11"/>
     </row>
     <row r="134">
-      <c r="C134" s="12"/>
+      <c r="C134" s="11"/>
     </row>
     <row r="135">
-      <c r="C135" s="12"/>
+      <c r="C135" s="11"/>
     </row>
     <row r="136">
-      <c r="C136" s="12"/>
+      <c r="C136" s="11"/>
     </row>
     <row r="137">
-      <c r="C137" s="12"/>
+      <c r="C137" s="11"/>
     </row>
     <row r="138">
-      <c r="C138" s="12"/>
+      <c r="C138" s="11"/>
     </row>
     <row r="139">
-      <c r="C139" s="12"/>
+      <c r="C139" s="11"/>
     </row>
     <row r="140">
-      <c r="C140" s="12"/>
+      <c r="C140" s="11"/>
     </row>
     <row r="141">
-      <c r="C141" s="12"/>
+      <c r="C141" s="11"/>
     </row>
     <row r="142">
-      <c r="C142" s="12"/>
+      <c r="C142" s="11"/>
     </row>
     <row r="143">
-      <c r="C143" s="12"/>
+      <c r="C143" s="11"/>
     </row>
     <row r="144">
-      <c r="C144" s="12"/>
+      <c r="C144" s="11"/>
     </row>
     <row r="145">
-      <c r="C145" s="12"/>
+      <c r="C145" s="11"/>
     </row>
     <row r="146">
-      <c r="C146" s="12"/>
+      <c r="C146" s="11"/>
     </row>
     <row r="147">
-      <c r="C147" s="12"/>
+      <c r="C147" s="11"/>
     </row>
     <row r="148">
-      <c r="C148" s="12"/>
+      <c r="C148" s="11"/>
     </row>
     <row r="149">
-      <c r="C149" s="12"/>
+      <c r="C149" s="11"/>
     </row>
     <row r="150">
-      <c r="C150" s="12"/>
+      <c r="C150" s="11"/>
     </row>
     <row r="151">
-      <c r="C151" s="12"/>
+      <c r="C151" s="11"/>
     </row>
     <row r="152">
-      <c r="C152" s="12"/>
+      <c r="C152" s="11"/>
     </row>
     <row r="153">
-      <c r="C153" s="12"/>
+      <c r="C153" s="11"/>
     </row>
     <row r="154">
-      <c r="C154" s="12"/>
+      <c r="C154" s="11"/>
     </row>
     <row r="155">
-      <c r="C155" s="12"/>
+      <c r="C155" s="11"/>
     </row>
     <row r="156">
-      <c r="C156" s="12"/>
+      <c r="C156" s="11"/>
     </row>
     <row r="157">
-      <c r="C157" s="12"/>
+      <c r="C157" s="11"/>
     </row>
     <row r="158">
-      <c r="C158" s="12"/>
+      <c r="C158" s="11"/>
     </row>
     <row r="159">
-      <c r="C159" s="12"/>
+      <c r="C159" s="11"/>
     </row>
     <row r="160">
-      <c r="C160" s="12"/>
+      <c r="C160" s="11"/>
     </row>
     <row r="161">
-      <c r="C161" s="12"/>
+      <c r="C161" s="11"/>
     </row>
     <row r="162">
-      <c r="C162" s="12"/>
+      <c r="C162" s="11"/>
     </row>
     <row r="163">
-      <c r="C163" s="12"/>
+      <c r="C163" s="11"/>
     </row>
     <row r="164">
-      <c r="C164" s="12"/>
+      <c r="C164" s="11"/>
     </row>
     <row r="165">
-      <c r="C165" s="12"/>
+      <c r="C165" s="11"/>
     </row>
     <row r="166">
-      <c r="C166" s="12"/>
+      <c r="C166" s="11"/>
     </row>
     <row r="167">
-      <c r="C167" s="12"/>
+      <c r="C167" s="11"/>
     </row>
     <row r="168">
-      <c r="C168" s="12"/>
+      <c r="C168" s="11"/>
     </row>
     <row r="169">
-      <c r="C169" s="12"/>
+      <c r="C169" s="11"/>
     </row>
     <row r="170">
-      <c r="C170" s="12"/>
+      <c r="C170" s="11"/>
     </row>
     <row r="171">
-      <c r="C171" s="12"/>
+      <c r="C171" s="11"/>
     </row>
     <row r="172">
-      <c r="C172" s="12"/>
+      <c r="C172" s="11"/>
     </row>
     <row r="173">
-      <c r="C173" s="12"/>
+      <c r="C173" s="11"/>
     </row>
     <row r="174">
-      <c r="C174" s="12"/>
+      <c r="C174" s="11"/>
     </row>
     <row r="175">
-      <c r="C175" s="12"/>
+      <c r="C175" s="11"/>
     </row>
     <row r="176">
-      <c r="C176" s="12"/>
+      <c r="C176" s="11"/>
     </row>
     <row r="177">
-      <c r="C177" s="12"/>
+      <c r="C177" s="11"/>
     </row>
     <row r="178">
-      <c r="C178" s="12"/>
+      <c r="C178" s="11"/>
     </row>
     <row r="179">
-      <c r="C179" s="12"/>
+      <c r="C179" s="11"/>
     </row>
     <row r="180">
-      <c r="C180" s="12"/>
+      <c r="C180" s="11"/>
     </row>
     <row r="181">
-      <c r="C181" s="12"/>
+      <c r="C181" s="11"/>
     </row>
     <row r="182">
-      <c r="C182" s="12"/>
+      <c r="C182" s="11"/>
     </row>
     <row r="183">
-      <c r="C183" s="12"/>
+      <c r="C183" s="11"/>
     </row>
     <row r="184">
-      <c r="C184" s="12"/>
+      <c r="C184" s="11"/>
     </row>
     <row r="185">
-      <c r="C185" s="12"/>
+      <c r="C185" s="11"/>
     </row>
     <row r="186">
-      <c r="C186" s="12"/>
+      <c r="C186" s="11"/>
     </row>
     <row r="187">
-      <c r="C187" s="12"/>
+      <c r="C187" s="11"/>
     </row>
     <row r="188">
-      <c r="C188" s="12"/>
+      <c r="C188" s="11"/>
     </row>
     <row r="189">
-      <c r="C189" s="12"/>
+      <c r="C189" s="11"/>
     </row>
     <row r="190">
-      <c r="C190" s="12"/>
+      <c r="C190" s="11"/>
     </row>
     <row r="191">
-      <c r="C191" s="12"/>
+      <c r="C191" s="11"/>
     </row>
     <row r="192">
-      <c r="C192" s="12"/>
+      <c r="C192" s="11"/>
     </row>
     <row r="193">
-      <c r="C193" s="12"/>
+      <c r="C193" s="11"/>
     </row>
     <row r="194">
-      <c r="C194" s="12"/>
+      <c r="C194" s="11"/>
     </row>
     <row r="195">
-      <c r="C195" s="12"/>
+      <c r="C195" s="11"/>
     </row>
     <row r="196">
-      <c r="C196" s="12"/>
+      <c r="C196" s="11"/>
     </row>
     <row r="197">
-      <c r="C197" s="12"/>
+      <c r="C197" s="11"/>
     </row>
     <row r="198">
-      <c r="C198" s="12"/>
+      <c r="C198" s="11"/>
     </row>
     <row r="199">
-      <c r="C199" s="12"/>
+      <c r="C199" s="11"/>
     </row>
     <row r="200">
-      <c r="C200" s="12"/>
+      <c r="C200" s="11"/>
     </row>
     <row r="201">
-      <c r="C201" s="12"/>
+      <c r="C201" s="11"/>
     </row>
     <row r="202">
-      <c r="C202" s="12"/>
+      <c r="C202" s="11"/>
     </row>
     <row r="203">
-      <c r="C203" s="12"/>
+      <c r="C203" s="11"/>
     </row>
     <row r="204">
-      <c r="C204" s="12"/>
+      <c r="C204" s="11"/>
     </row>
     <row r="205">
-      <c r="C205" s="12"/>
+      <c r="C205" s="11"/>
     </row>
     <row r="206">
-      <c r="C206" s="12"/>
+      <c r="C206" s="11"/>
     </row>
     <row r="207">
-      <c r="C207" s="12"/>
+      <c r="C207" s="11"/>
     </row>
     <row r="208">
-      <c r="C208" s="12"/>
+      <c r="C208" s="11"/>
     </row>
     <row r="209">
-      <c r="C209" s="12"/>
+      <c r="C209" s="11"/>
     </row>
     <row r="210">
-      <c r="C210" s="12"/>
+      <c r="C210" s="11"/>
     </row>
     <row r="211">
-      <c r="C211" s="12"/>
+      <c r="C211" s="11"/>
     </row>
     <row r="212">
-      <c r="C212" s="12"/>
+      <c r="C212" s="11"/>
     </row>
     <row r="213">
-      <c r="C213" s="12"/>
+      <c r="C213" s="11"/>
     </row>
     <row r="214">
-      <c r="C214" s="12"/>
+      <c r="C214" s="11"/>
     </row>
     <row r="215">
-      <c r="C215" s="12"/>
+      <c r="C215" s="11"/>
     </row>
     <row r="216">
-      <c r="C216" s="12"/>
+      <c r="C216" s="11"/>
     </row>
     <row r="217">
-      <c r="C217" s="12"/>
+      <c r="C217" s="11"/>
     </row>
     <row r="218">
-      <c r="C218" s="12"/>
+      <c r="C218" s="11"/>
     </row>
     <row r="219">
-      <c r="C219" s="12"/>
+      <c r="C219" s="11"/>
     </row>
     <row r="220">
-      <c r="C220" s="12"/>
+      <c r="C220" s="11"/>
     </row>
     <row r="221">
-      <c r="C221" s="12"/>
+      <c r="C221" s="11"/>
     </row>
     <row r="222">
-      <c r="C222" s="12"/>
+      <c r="C222" s="11"/>
     </row>
     <row r="223">
-      <c r="C223" s="12"/>
+      <c r="C223" s="11"/>
     </row>
     <row r="224">
-      <c r="C224" s="12"/>
+      <c r="C224" s="11"/>
     </row>
     <row r="225">
-      <c r="C225" s="12"/>
+      <c r="C225" s="11"/>
     </row>
     <row r="226">
-      <c r="C226" s="12"/>
+      <c r="C226" s="11"/>
     </row>
     <row r="227">
-      <c r="C227" s="12"/>
+      <c r="C227" s="11"/>
     </row>
     <row r="228">
-      <c r="C228" s="12"/>
+      <c r="C228" s="11"/>
     </row>
     <row r="229">
-      <c r="C229" s="12"/>
+      <c r="C229" s="11"/>
     </row>
     <row r="230">
-      <c r="C230" s="12"/>
+      <c r="C230" s="11"/>
     </row>
     <row r="231">
-      <c r="C231" s="12"/>
+      <c r="C231" s="11"/>
     </row>
     <row r="232">
-      <c r="C232" s="12"/>
+      <c r="C232" s="11"/>
     </row>
     <row r="233">
-      <c r="C233" s="12"/>
+      <c r="C233" s="11"/>
     </row>
     <row r="234">
-      <c r="C234" s="12"/>
+      <c r="C234" s="11"/>
     </row>
     <row r="235">
-      <c r="C235" s="12"/>
+      <c r="C235" s="11"/>
     </row>
     <row r="236">
-      <c r="C236" s="12"/>
+      <c r="C236" s="11"/>
     </row>
     <row r="237">
-      <c r="C237" s="12"/>
+      <c r="C237" s="11"/>
     </row>
     <row r="238">
-      <c r="C238" s="12"/>
+      <c r="C238" s="11"/>
     </row>
     <row r="239">
-      <c r="C239" s="12"/>
+      <c r="C239" s="11"/>
     </row>
     <row r="240">
-      <c r="C240" s="12"/>
+      <c r="C240" s="11"/>
     </row>
     <row r="241">
-      <c r="C241" s="12"/>
+      <c r="C241" s="11"/>
     </row>
     <row r="242">
-      <c r="C242" s="12"/>
+      <c r="C242" s="11"/>
     </row>
     <row r="243">
-      <c r="C243" s="12"/>
+      <c r="C243" s="11"/>
     </row>
     <row r="244">
-      <c r="C244" s="12"/>
+      <c r="C244" s="11"/>
     </row>
     <row r="245">
-      <c r="C245" s="12"/>
+      <c r="C245" s="11"/>
     </row>
     <row r="246">
-      <c r="C246" s="12"/>
+      <c r="C246" s="11"/>
     </row>
     <row r="247">
-      <c r="C247" s="12"/>
+      <c r="C247" s="11"/>
     </row>
     <row r="248">
-      <c r="C248" s="12"/>
+      <c r="C248" s="11"/>
     </row>
     <row r="249">
-      <c r="C249" s="12"/>
+      <c r="C249" s="11"/>
     </row>
     <row r="250">
-      <c r="C250" s="12"/>
+      <c r="C250" s="11"/>
     </row>
     <row r="251">
-      <c r="C251" s="12"/>
+      <c r="C251" s="11"/>
     </row>
     <row r="252">
-      <c r="C252" s="12"/>
+      <c r="C252" s="11"/>
     </row>
     <row r="253">
-      <c r="C253" s="12"/>
+      <c r="C253" s="11"/>
     </row>
     <row r="254">
-      <c r="C254" s="12"/>
+      <c r="C254" s="11"/>
     </row>
     <row r="255">
-      <c r="C255" s="12"/>
+      <c r="C255" s="11"/>
     </row>
     <row r="256">
-      <c r="C256" s="12"/>
+      <c r="C256" s="11"/>
     </row>
     <row r="257">
-      <c r="C257" s="12"/>
+      <c r="C257" s="11"/>
     </row>
     <row r="258">
-      <c r="C258" s="12"/>
+      <c r="C258" s="11"/>
     </row>
     <row r="259">
-      <c r="C259" s="12"/>
+      <c r="C259" s="11"/>
     </row>
     <row r="260">
-      <c r="C260" s="12"/>
+      <c r="C260" s="11"/>
     </row>
     <row r="261">
-      <c r="C261" s="12"/>
+      <c r="C261" s="11"/>
     </row>
     <row r="262">
-      <c r="C262" s="12"/>
+      <c r="C262" s="11"/>
     </row>
     <row r="263">
-      <c r="C263" s="12"/>
+      <c r="C263" s="11"/>
     </row>
     <row r="264">
-      <c r="C264" s="12"/>
+      <c r="C264" s="11"/>
     </row>
     <row r="265">
-      <c r="C265" s="12"/>
+      <c r="C265" s="11"/>
     </row>
     <row r="266">
-      <c r="C266" s="12"/>
+      <c r="C266" s="11"/>
     </row>
     <row r="267">
-      <c r="C267" s="12"/>
+      <c r="C267" s="11"/>
     </row>
     <row r="268">
-      <c r="C268" s="12"/>
+      <c r="C268" s="11"/>
     </row>
     <row r="269">
-      <c r="C269" s="12"/>
+      <c r="C269" s="11"/>
     </row>
     <row r="270">
-      <c r="C270" s="12"/>
+      <c r="C270" s="11"/>
     </row>
     <row r="271">
-      <c r="C271" s="12"/>
+      <c r="C271" s="11"/>
     </row>
     <row r="272">
-      <c r="C272" s="12"/>
+      <c r="C272" s="11"/>
     </row>
     <row r="273">
-      <c r="C273" s="12"/>
+      <c r="C273" s="11"/>
     </row>
     <row r="274">
-      <c r="C274" s="12"/>
+      <c r="C274" s="11"/>
     </row>
     <row r="275">
-      <c r="C275" s="12"/>
+      <c r="C275" s="11"/>
     </row>
     <row r="276">
-      <c r="C276" s="12"/>
+      <c r="C276" s="11"/>
     </row>
     <row r="277">
-      <c r="C277" s="12"/>
+      <c r="C277" s="11"/>
     </row>
     <row r="278">
-      <c r="C278" s="12"/>
+      <c r="C278" s="11"/>
     </row>
     <row r="279">
-      <c r="C279" s="12"/>
+      <c r="C279" s="11"/>
     </row>
     <row r="280">
-      <c r="C280" s="12"/>
+      <c r="C280" s="11"/>
     </row>
     <row r="281">
-      <c r="C281" s="12"/>
+      <c r="C281" s="11"/>
     </row>
     <row r="282">
-      <c r="C282" s="12"/>
+      <c r="C282" s="11"/>
     </row>
     <row r="283">
-      <c r="C283" s="12"/>
+      <c r="C283" s="11"/>
     </row>
     <row r="284">
-      <c r="C284" s="12"/>
+      <c r="C284" s="11"/>
     </row>
     <row r="285">
-      <c r="C285" s="12"/>
+      <c r="C285" s="11"/>
     </row>
     <row r="286">
-      <c r="C286" s="12"/>
+      <c r="C286" s="11"/>
     </row>
     <row r="287">
-      <c r="C287" s="12"/>
+      <c r="C287" s="11"/>
     </row>
     <row r="288">
-      <c r="C288" s="12"/>
+      <c r="C288" s="11"/>
     </row>
     <row r="289">
-      <c r="C289" s="12"/>
+      <c r="C289" s="11"/>
     </row>
     <row r="290">
-      <c r="C290" s="12"/>
+      <c r="C290" s="11"/>
     </row>
     <row r="291">
-      <c r="C291" s="12"/>
+      <c r="C291" s="11"/>
     </row>
     <row r="292">
-      <c r="C292" s="12"/>
+      <c r="C292" s="11"/>
     </row>
     <row r="293">
-      <c r="C293" s="12"/>
+      <c r="C293" s="11"/>
     </row>
     <row r="294">
-      <c r="C294" s="12"/>
+      <c r="C294" s="11"/>
     </row>
     <row r="295">
-      <c r="C295" s="12"/>
+      <c r="C295" s="11"/>
     </row>
     <row r="296">
-      <c r="C296" s="12"/>
+      <c r="C296" s="11"/>
     </row>
     <row r="297">
-      <c r="C297" s="12"/>
+      <c r="C297" s="11"/>
     </row>
     <row r="298">
-      <c r="C298" s="12"/>
+      <c r="C298" s="11"/>
     </row>
     <row r="299">
-      <c r="C299" s="12"/>
+      <c r="C299" s="11"/>
     </row>
     <row r="300">
-      <c r="C300" s="12"/>
+      <c r="C300" s="11"/>
     </row>
     <row r="301">
-      <c r="C301" s="12"/>
+      <c r="C301" s="11"/>
     </row>
     <row r="302">
-      <c r="C302" s="12"/>
+      <c r="C302" s="11"/>
     </row>
     <row r="303">
-      <c r="C303" s="12"/>
+      <c r="C303" s="11"/>
     </row>
     <row r="304">
-      <c r="C304" s="12"/>
+      <c r="C304" s="11"/>
     </row>
     <row r="305">
-      <c r="C305" s="12"/>
+      <c r="C305" s="11"/>
     </row>
     <row r="306">
-      <c r="C306" s="12"/>
+      <c r="C306" s="11"/>
     </row>
     <row r="307">
-      <c r="C307" s="12"/>
+      <c r="C307" s="11"/>
     </row>
     <row r="308">
-      <c r="C308" s="12"/>
+      <c r="C308" s="11"/>
     </row>
     <row r="309">
-      <c r="C309" s="12"/>
+      <c r="C309" s="11"/>
     </row>
     <row r="310">
-      <c r="C310" s="12"/>
+      <c r="C310" s="11"/>
     </row>
     <row r="311">
-      <c r="C311" s="12"/>
+      <c r="C311" s="11"/>
     </row>
     <row r="312">
-      <c r="C312" s="12"/>
+      <c r="C312" s="11"/>
     </row>
     <row r="313">
-      <c r="C313" s="12"/>
+      <c r="C313" s="11"/>
     </row>
     <row r="314">
-      <c r="C314" s="12"/>
+      <c r="C314" s="11"/>
     </row>
     <row r="315">
-      <c r="C315" s="12"/>
+      <c r="C315" s="11"/>
     </row>
     <row r="316">
-      <c r="C316" s="12"/>
+      <c r="C316" s="11"/>
     </row>
     <row r="317">
-      <c r="C317" s="12"/>
+      <c r="C317" s="11"/>
     </row>
     <row r="318">
-      <c r="C318" s="12"/>
+      <c r="C318" s="11"/>
     </row>
     <row r="319">
-      <c r="C319" s="12"/>
+      <c r="C319" s="11"/>
     </row>
     <row r="320">
-      <c r="C320" s="12"/>
+      <c r="C320" s="11"/>
     </row>
     <row r="321">
-      <c r="C321" s="12"/>
+      <c r="C321" s="11"/>
     </row>
     <row r="322">
-      <c r="C322" s="12"/>
+      <c r="C322" s="11"/>
     </row>
     <row r="323">
-      <c r="C323" s="12"/>
+      <c r="C323" s="11"/>
     </row>
     <row r="324">
-      <c r="C324" s="12"/>
+      <c r="C324" s="11"/>
     </row>
     <row r="325">
-      <c r="C325" s="12"/>
+      <c r="C325" s="11"/>
     </row>
     <row r="326">
-      <c r="C326" s="12"/>
+      <c r="C326" s="11"/>
     </row>
     <row r="327">
-      <c r="C327" s="12"/>
+      <c r="C327" s="11"/>
     </row>
     <row r="328">
-      <c r="C328" s="12"/>
+      <c r="C328" s="11"/>
     </row>
     <row r="329">
-      <c r="C329" s="12"/>
+      <c r="C329" s="11"/>
     </row>
     <row r="330">
-      <c r="C330" s="12"/>
+      <c r="C330" s="11"/>
     </row>
     <row r="331">
-      <c r="C331" s="12"/>
+      <c r="C331" s="11"/>
     </row>
     <row r="332">
-      <c r="C332" s="12"/>
+      <c r="C332" s="11"/>
     </row>
     <row r="333">
-      <c r="C333" s="12"/>
+      <c r="C333" s="11"/>
     </row>
     <row r="334">
-      <c r="C334" s="12"/>
+      <c r="C334" s="11"/>
     </row>
     <row r="335">
-      <c r="C335" s="12"/>
+      <c r="C335" s="11"/>
     </row>
     <row r="336">
-      <c r="C336" s="12"/>
+      <c r="C336" s="11"/>
     </row>
     <row r="337">
-      <c r="C337" s="12"/>
+      <c r="C337" s="11"/>
     </row>
     <row r="338">
-      <c r="C338" s="12"/>
+      <c r="C338" s="11"/>
     </row>
     <row r="339">
-      <c r="C339" s="12"/>
+      <c r="C339" s="11"/>
     </row>
     <row r="340">
-      <c r="C340" s="12"/>
+      <c r="C340" s="11"/>
     </row>
     <row r="341">
-      <c r="C341" s="12"/>
+      <c r="C341" s="11"/>
     </row>
     <row r="342">
-      <c r="C342" s="12"/>
+      <c r="C342" s="11"/>
     </row>
     <row r="343">
-      <c r="C343" s="12"/>
+      <c r="C343" s="11"/>
     </row>
     <row r="344">
-      <c r="C344" s="12"/>
+      <c r="C344" s="11"/>
     </row>
     <row r="345">
-      <c r="C345" s="12"/>
+      <c r="C345" s="11"/>
     </row>
     <row r="346">
-      <c r="C346" s="12"/>
+      <c r="C346" s="11"/>
     </row>
     <row r="347">
-      <c r="C347" s="12"/>
+      <c r="C347" s="11"/>
     </row>
     <row r="348">
-      <c r="C348" s="12"/>
+      <c r="C348" s="11"/>
     </row>
     <row r="349">
-      <c r="C349" s="12"/>
+      <c r="C349" s="11"/>
     </row>
     <row r="350">
-      <c r="C350" s="12"/>
+      <c r="C350" s="11"/>
     </row>
     <row r="351">
-      <c r="C351" s="12"/>
+      <c r="C351" s="11"/>
     </row>
     <row r="352">
-      <c r="C352" s="12"/>
+      <c r="C352" s="11"/>
     </row>
     <row r="353">
-      <c r="C353" s="12"/>
+      <c r="C353" s="11"/>
     </row>
     <row r="354">
-      <c r="C354" s="12"/>
+      <c r="C354" s="11"/>
     </row>
     <row r="355">
-      <c r="C355" s="12"/>
+      <c r="C355" s="11"/>
     </row>
     <row r="356">
-      <c r="C356" s="12"/>
+      <c r="C356" s="11"/>
     </row>
     <row r="357">
-      <c r="C357" s="12"/>
+      <c r="C357" s="11"/>
     </row>
     <row r="358">
-      <c r="C358" s="12"/>
+      <c r="C358" s="11"/>
     </row>
     <row r="359">
-      <c r="C359" s="12"/>
+      <c r="C359" s="11"/>
     </row>
     <row r="360">
-      <c r="C360" s="12"/>
+      <c r="C360" s="11"/>
     </row>
     <row r="361">
-      <c r="C361" s="12"/>
+      <c r="C361" s="11"/>
     </row>
     <row r="362">
-      <c r="C362" s="12"/>
+      <c r="C362" s="11"/>
     </row>
     <row r="363">
-      <c r="C363" s="12"/>
+      <c r="C363" s="11"/>
     </row>
     <row r="364">
-      <c r="C364" s="12"/>
+      <c r="C364" s="11"/>
     </row>
     <row r="365">
-      <c r="C365" s="12"/>
+      <c r="C365" s="11"/>
     </row>
     <row r="366">
-      <c r="C366" s="12"/>
+      <c r="C366" s="11"/>
     </row>
     <row r="367">
-      <c r="C367" s="12"/>
+      <c r="C367" s="11"/>
     </row>
     <row r="368">
-      <c r="C368" s="12"/>
+      <c r="C368" s="11"/>
     </row>
     <row r="369">
-      <c r="C369" s="12"/>
+      <c r="C369" s="11"/>
     </row>
     <row r="370">
-      <c r="C370" s="12"/>
+      <c r="C370" s="11"/>
     </row>
     <row r="371">
-      <c r="C371" s="12"/>
+      <c r="C371" s="11"/>
     </row>
     <row r="372">
-      <c r="C372" s="12"/>
+      <c r="C372" s="11"/>
     </row>
     <row r="373">
-      <c r="C373" s="12"/>
+      <c r="C373" s="11"/>
     </row>
     <row r="374">
-      <c r="C374" s="12"/>
+      <c r="C374" s="11"/>
     </row>
     <row r="375">
-      <c r="C375" s="12"/>
+      <c r="C375" s="11"/>
     </row>
     <row r="376">
-      <c r="C376" s="12"/>
+      <c r="C376" s="11"/>
     </row>
     <row r="377">
-      <c r="C377" s="12"/>
+      <c r="C377" s="11"/>
     </row>
     <row r="378">
-      <c r="C378" s="12"/>
+      <c r="C378" s="11"/>
     </row>
     <row r="379">
-      <c r="C379" s="12"/>
+      <c r="C379" s="11"/>
     </row>
     <row r="380">
-      <c r="C380" s="12"/>
+      <c r="C380" s="11"/>
     </row>
     <row r="381">
-      <c r="C381" s="12"/>
+      <c r="C381" s="11"/>
     </row>
     <row r="382">
-      <c r="C382" s="12"/>
+      <c r="C382" s="11"/>
     </row>
     <row r="383">
-      <c r="C383" s="12"/>
+      <c r="C383" s="11"/>
     </row>
     <row r="384">
-      <c r="C384" s="12"/>
+      <c r="C384" s="11"/>
     </row>
     <row r="385">
-      <c r="C385" s="12"/>
+      <c r="C385" s="11"/>
     </row>
     <row r="386">
-      <c r="C386" s="12"/>
+      <c r="C386" s="11"/>
     </row>
     <row r="387">
-      <c r="C387" s="12"/>
+      <c r="C387" s="11"/>
     </row>
     <row r="388">
-      <c r="C388" s="12"/>
+      <c r="C388" s="11"/>
     </row>
     <row r="389">
-      <c r="C389" s="12"/>
+      <c r="C389" s="11"/>
     </row>
     <row r="390">
-      <c r="C390" s="12"/>
+      <c r="C390" s="11"/>
     </row>
     <row r="391">
-      <c r="C391" s="12"/>
+      <c r="C391" s="11"/>
     </row>
     <row r="392">
-      <c r="C392" s="12"/>
+      <c r="C392" s="11"/>
     </row>
     <row r="393">
-      <c r="C393" s="12"/>
+      <c r="C393" s="11"/>
     </row>
     <row r="394">
-      <c r="C394" s="12"/>
+      <c r="C394" s="11"/>
     </row>
     <row r="395">
-      <c r="C395" s="12"/>
+      <c r="C395" s="11"/>
     </row>
     <row r="396">
-      <c r="C396" s="12"/>
+      <c r="C396" s="11"/>
     </row>
     <row r="397">
-      <c r="C397" s="12"/>
+      <c r="C397" s="11"/>
     </row>
     <row r="398">
-      <c r="C398" s="12"/>
+      <c r="C398" s="11"/>
     </row>
     <row r="399">
-      <c r="C399" s="12"/>
+      <c r="C399" s="11"/>
     </row>
     <row r="400">
-      <c r="C400" s="12"/>
+      <c r="C400" s="11"/>
     </row>
     <row r="401">
-      <c r="C401" s="12"/>
+      <c r="C401" s="11"/>
     </row>
     <row r="402">
-      <c r="C402" s="12"/>
+      <c r="C402" s="11"/>
     </row>
     <row r="403">
-      <c r="C403" s="12"/>
+      <c r="C403" s="11"/>
     </row>
     <row r="404">
-      <c r="C404" s="12"/>
+      <c r="C404" s="11"/>
     </row>
     <row r="405">
-      <c r="C405" s="12"/>
+      <c r="C405" s="11"/>
     </row>
     <row r="406">
-      <c r="C406" s="12"/>
+      <c r="C406" s="11"/>
     </row>
     <row r="407">
-      <c r="C407" s="12"/>
+      <c r="C407" s="11"/>
     </row>
     <row r="408">
-      <c r="C408" s="12"/>
+      <c r="C408" s="11"/>
     </row>
     <row r="409">
-      <c r="C409" s="12"/>
+      <c r="C409" s="11"/>
     </row>
     <row r="410">
-      <c r="C410" s="12"/>
+      <c r="C410" s="11"/>
     </row>
     <row r="411">
-      <c r="C411" s="12"/>
+      <c r="C411" s="11"/>
     </row>
     <row r="412">
-      <c r="C412" s="12"/>
+      <c r="C412" s="11"/>
     </row>
     <row r="413">
-      <c r="C413" s="12"/>
+      <c r="C413" s="11"/>
     </row>
     <row r="414">
-      <c r="C414" s="12"/>
+      <c r="C414" s="11"/>
     </row>
     <row r="415">
-      <c r="C415" s="12"/>
+      <c r="C415" s="11"/>
     </row>
     <row r="416">
-      <c r="C416" s="12"/>
+      <c r="C416" s="11"/>
     </row>
     <row r="417">
-      <c r="C417" s="12"/>
+      <c r="C417" s="11"/>
     </row>
     <row r="418">
-      <c r="C418" s="12"/>
+      <c r="C418" s="11"/>
     </row>
     <row r="419">
-      <c r="C419" s="12"/>
+      <c r="C419" s="11"/>
     </row>
     <row r="420">
-      <c r="C420" s="12"/>
+      <c r="C420" s="11"/>
     </row>
     <row r="421">
-      <c r="C421" s="12"/>
+      <c r="C421" s="11"/>
     </row>
     <row r="422">
-      <c r="C422" s="12"/>
+      <c r="C422" s="11"/>
     </row>
     <row r="423">
-      <c r="C423" s="12"/>
+      <c r="C423" s="11"/>
     </row>
     <row r="424">
-      <c r="C424" s="12"/>
+      <c r="C424" s="11"/>
     </row>
     <row r="425">
-      <c r="C425" s="12"/>
+      <c r="C425" s="11"/>
     </row>
     <row r="426">
-      <c r="C426" s="12"/>
+      <c r="C426" s="11"/>
     </row>
     <row r="427">
-      <c r="C427" s="12"/>
+      <c r="C427" s="11"/>
     </row>
     <row r="428">
-      <c r="C428" s="12"/>
+      <c r="C428" s="11"/>
     </row>
     <row r="429">
-      <c r="C429" s="12"/>
+      <c r="C429" s="11"/>
     </row>
     <row r="430">
-      <c r="C430" s="12"/>
+      <c r="C430" s="11"/>
     </row>
     <row r="431">
-      <c r="C431" s="12"/>
+      <c r="C431" s="11"/>
     </row>
     <row r="432">
-      <c r="C432" s="12"/>
+      <c r="C432" s="11"/>
     </row>
     <row r="433">
-      <c r="C433" s="12"/>
+      <c r="C433" s="11"/>
     </row>
     <row r="434">
-      <c r="C434" s="12"/>
+      <c r="C434" s="11"/>
     </row>
     <row r="435">
-      <c r="C435" s="12"/>
+      <c r="C435" s="11"/>
     </row>
     <row r="436">
-      <c r="C436" s="12"/>
+      <c r="C436" s="11"/>
     </row>
     <row r="437">
-      <c r="C437" s="12"/>
+      <c r="C437" s="11"/>
     </row>
     <row r="438">
-      <c r="C438" s="12"/>
+      <c r="C438" s="11"/>
     </row>
     <row r="439">
-      <c r="C439" s="12"/>
+      <c r="C439" s="11"/>
     </row>
     <row r="440">
-      <c r="C440" s="12"/>
+      <c r="C440" s="11"/>
     </row>
     <row r="441">
-      <c r="C441" s="12"/>
+      <c r="C441" s="11"/>
     </row>
     <row r="442">
-      <c r="C442" s="12"/>
+      <c r="C442" s="11"/>
     </row>
     <row r="443">
-      <c r="C443" s="12"/>
+      <c r="C443" s="11"/>
     </row>
     <row r="444">
-      <c r="C444" s="12"/>
+      <c r="C444" s="11"/>
     </row>
     <row r="445">
-      <c r="C445" s="12"/>
+      <c r="C445" s="11"/>
     </row>
     <row r="446">
-      <c r="C446" s="12"/>
+      <c r="C446" s="11"/>
     </row>
     <row r="447">
-      <c r="C447" s="12"/>
+      <c r="C447" s="11"/>
     </row>
     <row r="448">
-      <c r="C448" s="12"/>
+      <c r="C448" s="11"/>
     </row>
     <row r="449">
-      <c r="C449" s="12"/>
+      <c r="C449" s="11"/>
     </row>
     <row r="450">
-      <c r="C450" s="12"/>
+      <c r="C450" s="11"/>
     </row>
     <row r="451">
-      <c r="C451" s="12"/>
+      <c r="C451" s="11"/>
     </row>
     <row r="452">
-      <c r="C452" s="12"/>
+      <c r="C452" s="11"/>
     </row>
     <row r="453">
-      <c r="C453" s="12"/>
+      <c r="C453" s="11"/>
     </row>
     <row r="454">
-      <c r="C454" s="12"/>
+      <c r="C454" s="11"/>
     </row>
     <row r="455">
-      <c r="C455" s="12"/>
+      <c r="C455" s="11"/>
     </row>
     <row r="456">
-      <c r="C456" s="12"/>
+      <c r="C456" s="11"/>
     </row>
     <row r="457">
-      <c r="C457" s="12"/>
+      <c r="C457" s="11"/>
     </row>
     <row r="458">
-      <c r="C458" s="12"/>
+      <c r="C458" s="11"/>
     </row>
     <row r="459">
-      <c r="C459" s="12"/>
+      <c r="C459" s="11"/>
     </row>
     <row r="460">
-      <c r="C460" s="12"/>
+      <c r="C460" s="11"/>
     </row>
     <row r="461">
-      <c r="C461" s="12"/>
+      <c r="C461" s="11"/>
     </row>
     <row r="462">
-      <c r="C462" s="12"/>
+      <c r="C462" s="11"/>
     </row>
     <row r="463">
-      <c r="C463" s="12"/>
+      <c r="C463" s="11"/>
     </row>
     <row r="464">
-      <c r="C464" s="12"/>
+      <c r="C464" s="11"/>
     </row>
     <row r="465">
-      <c r="C465" s="12"/>
+      <c r="C465" s="11"/>
     </row>
     <row r="466">
-      <c r="C466" s="12"/>
+      <c r="C466" s="11"/>
     </row>
     <row r="467">
-      <c r="C467" s="12"/>
+      <c r="C467" s="11"/>
     </row>
     <row r="468">
-      <c r="C468" s="12"/>
+      <c r="C468" s="11"/>
     </row>
     <row r="469">
-      <c r="C469" s="12"/>
+      <c r="C469" s="11"/>
     </row>
     <row r="470">
-      <c r="C470" s="12"/>
+      <c r="C470" s="11"/>
     </row>
     <row r="471">
-      <c r="C471" s="12"/>
+      <c r="C471" s="11"/>
     </row>
     <row r="472">
-      <c r="C472" s="12"/>
+      <c r="C472" s="11"/>
     </row>
     <row r="473">
-      <c r="C473" s="12"/>
+      <c r="C473" s="11"/>
     </row>
     <row r="474">
-      <c r="C474" s="12"/>
+      <c r="C474" s="11"/>
     </row>
     <row r="475">
-      <c r="C475" s="12"/>
+      <c r="C475" s="11"/>
     </row>
     <row r="476">
-      <c r="C476" s="12"/>
+      <c r="C476" s="11"/>
     </row>
     <row r="477">
-      <c r="C477" s="12"/>
+      <c r="C477" s="11"/>
     </row>
     <row r="478">
-      <c r="C478" s="12"/>
+      <c r="C478" s="11"/>
     </row>
     <row r="479">
-      <c r="C479" s="12"/>
+      <c r="C479" s="11"/>
     </row>
     <row r="480">
-      <c r="C480" s="12"/>
+      <c r="C480" s="11"/>
     </row>
     <row r="481">
-      <c r="C481" s="12"/>
+      <c r="C481" s="11"/>
     </row>
     <row r="482">
-      <c r="C482" s="12"/>
+      <c r="C482" s="11"/>
     </row>
     <row r="483">
-      <c r="C483" s="12"/>
+      <c r="C483" s="11"/>
     </row>
     <row r="484">
-      <c r="C484" s="12"/>
+      <c r="C484" s="11"/>
     </row>
     <row r="485">
-      <c r="C485" s="12"/>
+      <c r="C485" s="11"/>
     </row>
     <row r="486">
-      <c r="C486" s="12"/>
+      <c r="C486" s="11"/>
     </row>
     <row r="487">
-      <c r="C487" s="12"/>
+      <c r="C487" s="11"/>
     </row>
     <row r="488">
-      <c r="C488" s="12"/>
+      <c r="C488" s="11"/>
     </row>
     <row r="489">
-      <c r="C489" s="12"/>
+      <c r="C489" s="11"/>
     </row>
     <row r="490">
-      <c r="C490" s="12"/>
+      <c r="C490" s="11"/>
     </row>
     <row r="491">
-      <c r="C491" s="12"/>
+      <c r="C491" s="11"/>
     </row>
     <row r="492">
-      <c r="C492" s="12"/>
+      <c r="C492" s="11"/>
     </row>
     <row r="493">
-      <c r="C493" s="12"/>
+      <c r="C493" s="11"/>
     </row>
     <row r="494">
-      <c r="C494" s="12"/>
+      <c r="C494" s="11"/>
     </row>
     <row r="495">
-      <c r="C495" s="12"/>
+      <c r="C495" s="11"/>
     </row>
     <row r="496">
-      <c r="C496" s="12"/>
+      <c r="C496" s="11"/>
     </row>
     <row r="497">
-      <c r="C497" s="12"/>
+      <c r="C497" s="11"/>
     </row>
     <row r="498">
-      <c r="C498" s="12"/>
+      <c r="C498" s="11"/>
     </row>
     <row r="499">
-      <c r="C499" s="12"/>
+      <c r="C499" s="11"/>
     </row>
     <row r="500">
-      <c r="C500" s="12"/>
+      <c r="C500" s="11"/>
     </row>
     <row r="501">
-      <c r="C501" s="12"/>
+      <c r="C501" s="11"/>
     </row>
     <row r="502">
-      <c r="C502" s="12"/>
+      <c r="C502" s="11"/>
     </row>
     <row r="503">
-      <c r="C503" s="12"/>
+      <c r="C503" s="11"/>
     </row>
     <row r="504">
-      <c r="C504" s="12"/>
+      <c r="C504" s="11"/>
     </row>
     <row r="505">
-      <c r="C505" s="12"/>
+      <c r="C505" s="11"/>
     </row>
     <row r="506">
-      <c r="C506" s="12"/>
+      <c r="C506" s="11"/>
     </row>
     <row r="507">
-      <c r="C507" s="12"/>
+      <c r="C507" s="11"/>
     </row>
     <row r="508">
-      <c r="C508" s="12"/>
+      <c r="C508" s="11"/>
     </row>
     <row r="509">
-      <c r="C509" s="12"/>
+      <c r="C509" s="11"/>
     </row>
     <row r="510">
-      <c r="C510" s="12"/>
+      <c r="C510" s="11"/>
     </row>
     <row r="511">
-      <c r="C511" s="12"/>
+      <c r="C511" s="11"/>
     </row>
     <row r="512">
-      <c r="C512" s="12"/>
+      <c r="C512" s="11"/>
     </row>
     <row r="513">
-      <c r="C513" s="12"/>
+      <c r="C513" s="11"/>
     </row>
     <row r="514">
-      <c r="C514" s="12"/>
+      <c r="C514" s="11"/>
     </row>
     <row r="515">
-      <c r="C515" s="12"/>
+      <c r="C515" s="11"/>
     </row>
     <row r="516">
-      <c r="C516" s="12"/>
+      <c r="C516" s="11"/>
     </row>
     <row r="517">
-      <c r="C517" s="12"/>
+      <c r="C517" s="11"/>
     </row>
     <row r="518">
-      <c r="C518" s="12"/>
+      <c r="C518" s="11"/>
     </row>
     <row r="519">
-      <c r="C519" s="12"/>
+      <c r="C519" s="11"/>
     </row>
     <row r="520">
-      <c r="C520" s="12"/>
+      <c r="C520" s="11"/>
     </row>
     <row r="521">
-      <c r="C521" s="12"/>
+      <c r="C521" s="11"/>
     </row>
     <row r="522">
-      <c r="C522" s="12"/>
+      <c r="C522" s="11"/>
     </row>
     <row r="523">
-      <c r="C523" s="12"/>
+      <c r="C523" s="11"/>
     </row>
     <row r="524">
-      <c r="C524" s="12"/>
+      <c r="C524" s="11"/>
     </row>
     <row r="525">
-      <c r="C525" s="12"/>
+      <c r="C525" s="11"/>
     </row>
     <row r="526">
-      <c r="C526" s="12"/>
+      <c r="C526" s="11"/>
     </row>
     <row r="527">
-      <c r="C527" s="12"/>
+      <c r="C527" s="11"/>
     </row>
     <row r="528">
-      <c r="C528" s="12"/>
+      <c r="C528" s="11"/>
     </row>
     <row r="529">
-      <c r="C529" s="12"/>
+      <c r="C529" s="11"/>
     </row>
     <row r="530">
-      <c r="C530" s="12"/>
+      <c r="C530" s="11"/>
     </row>
     <row r="531">
-      <c r="C531" s="12"/>
+      <c r="C531" s="11"/>
     </row>
     <row r="532">
-      <c r="C532" s="12"/>
+      <c r="C532" s="11"/>
     </row>
     <row r="533">
-      <c r="C533" s="12"/>
+      <c r="C533" s="11"/>
     </row>
     <row r="534">
-      <c r="C534" s="12"/>
+      <c r="C534" s="11"/>
     </row>
     <row r="535">
-      <c r="C535" s="12"/>
+      <c r="C535" s="11"/>
     </row>
     <row r="536">
-      <c r="C536" s="12"/>
+      <c r="C536" s="11"/>
     </row>
     <row r="537">
-      <c r="C537" s="12"/>
+      <c r="C537" s="11"/>
     </row>
     <row r="538">
-      <c r="C538" s="12"/>
+      <c r="C538" s="11"/>
     </row>
     <row r="539">
-      <c r="C539" s="12"/>
+      <c r="C539" s="11"/>
     </row>
     <row r="540">
-      <c r="C540" s="12"/>
+      <c r="C540" s="11"/>
     </row>
     <row r="541">
-      <c r="C541" s="12"/>
+      <c r="C541" s="11"/>
     </row>
     <row r="542">
-      <c r="C542" s="12"/>
+      <c r="C542" s="11"/>
     </row>
     <row r="543">
-      <c r="C543" s="12"/>
+      <c r="C543" s="11"/>
     </row>
     <row r="544">
-      <c r="C544" s="12"/>
+      <c r="C544" s="11"/>
     </row>
     <row r="545">
-      <c r="C545" s="12"/>
+      <c r="C545" s="11"/>
     </row>
     <row r="546">
-      <c r="C546" s="12"/>
+      <c r="C546" s="11"/>
     </row>
     <row r="547">
-      <c r="C547" s="12"/>
+      <c r="C547" s="11"/>
     </row>
     <row r="548">
-      <c r="C548" s="12"/>
+      <c r="C548" s="11"/>
     </row>
     <row r="549">
-      <c r="C549" s="12"/>
+      <c r="C549" s="11"/>
     </row>
     <row r="550">
-      <c r="C550" s="12"/>
+      <c r="C550" s="11"/>
     </row>
     <row r="551">
-      <c r="C551" s="12"/>
+      <c r="C551" s="11"/>
     </row>
     <row r="552">
-      <c r="C552" s="12"/>
+      <c r="C552" s="11"/>
     </row>
     <row r="553">
-      <c r="C553" s="12"/>
+      <c r="C553" s="11"/>
     </row>
     <row r="554">
-      <c r="C554" s="12"/>
+      <c r="C554" s="11"/>
     </row>
     <row r="555">
-      <c r="C555" s="12"/>
+      <c r="C555" s="11"/>
     </row>
     <row r="556">
-      <c r="C556" s="12"/>
+      <c r="C556" s="11"/>
     </row>
     <row r="557">
-      <c r="C557" s="12"/>
+      <c r="C557" s="11"/>
     </row>
     <row r="558">
-      <c r="C558" s="12"/>
+      <c r="C558" s="11"/>
     </row>
     <row r="559">
-      <c r="C559" s="12"/>
+      <c r="C559" s="11"/>
     </row>
     <row r="560">
-      <c r="C560" s="12"/>
+      <c r="C560" s="11"/>
     </row>
     <row r="561">
-      <c r="C561" s="12"/>
+      <c r="C561" s="11"/>
     </row>
     <row r="562">
-      <c r="C562" s="12"/>
+      <c r="C562" s="11"/>
     </row>
     <row r="563">
-      <c r="C563" s="12"/>
+      <c r="C563" s="11"/>
     </row>
     <row r="564">
-      <c r="C564" s="12"/>
+      <c r="C564" s="11"/>
     </row>
     <row r="565">
-      <c r="C565" s="12"/>
+      <c r="C565" s="11"/>
     </row>
     <row r="566">
-      <c r="C566" s="12"/>
+      <c r="C566" s="11"/>
     </row>
     <row r="567">
-      <c r="C567" s="12"/>
+      <c r="C567" s="11"/>
     </row>
     <row r="568">
-      <c r="C568" s="12"/>
+      <c r="C568" s="11"/>
     </row>
     <row r="569">
-      <c r="C569" s="12"/>
+      <c r="C569" s="11"/>
     </row>
     <row r="570">
-      <c r="C570" s="12"/>
+      <c r="C570" s="11"/>
     </row>
     <row r="571">
-      <c r="C571" s="12"/>
+      <c r="C571" s="11"/>
     </row>
     <row r="572">
-      <c r="C572" s="12"/>
+      <c r="C572" s="11"/>
     </row>
     <row r="573">
-      <c r="C573" s="12"/>
+      <c r="C573" s="11"/>
     </row>
     <row r="574">
-      <c r="C574" s="12"/>
+      <c r="C574" s="11"/>
     </row>
     <row r="575">
-      <c r="C575" s="12"/>
+      <c r="C575" s="11"/>
     </row>
     <row r="576">
-      <c r="C576" s="12"/>
+      <c r="C576" s="11"/>
     </row>
     <row r="577">
-      <c r="C577" s="12"/>
+      <c r="C577" s="11"/>
     </row>
     <row r="578">
-      <c r="C578" s="12"/>
+      <c r="C578" s="11"/>
     </row>
     <row r="579">
-      <c r="C579" s="12"/>
+      <c r="C579" s="11"/>
     </row>
     <row r="580">
-      <c r="C580" s="12"/>
+      <c r="C580" s="11"/>
     </row>
     <row r="581">
-      <c r="C581" s="12"/>
+      <c r="C581" s="11"/>
     </row>
     <row r="582">
-      <c r="C582" s="12"/>
+      <c r="C582" s="11"/>
     </row>
     <row r="583">
-      <c r="C583" s="12"/>
+      <c r="C583" s="11"/>
     </row>
     <row r="584">
-      <c r="C584" s="12"/>
+      <c r="C584" s="11"/>
     </row>
     <row r="585">
-      <c r="C585" s="12"/>
+      <c r="C585" s="11"/>
     </row>
     <row r="586">
-      <c r="C586" s="12"/>
+      <c r="C586" s="11"/>
     </row>
     <row r="587">
-      <c r="C587" s="12"/>
+      <c r="C587" s="11"/>
     </row>
     <row r="588">
-      <c r="C588" s="12"/>
+      <c r="C588" s="11"/>
     </row>
     <row r="589">
-      <c r="C589" s="12"/>
+      <c r="C589" s="11"/>
     </row>
     <row r="590">
-      <c r="C590" s="12"/>
+      <c r="C590" s="11"/>
     </row>
     <row r="591">
-      <c r="C591" s="12"/>
+      <c r="C591" s="11"/>
     </row>
     <row r="592">
-      <c r="C592" s="12"/>
+      <c r="C592" s="11"/>
     </row>
     <row r="593">
-      <c r="C593" s="12"/>
+      <c r="C593" s="11"/>
     </row>
     <row r="594">
-      <c r="C594" s="12"/>
+      <c r="C594" s="11"/>
     </row>
     <row r="595">
-      <c r="C595" s="12"/>
+      <c r="C595" s="11"/>
     </row>
     <row r="596">
-      <c r="C596" s="12"/>
+      <c r="C596" s="11"/>
     </row>
     <row r="597">
-      <c r="C597" s="12"/>
+      <c r="C597" s="11"/>
     </row>
     <row r="598">
-      <c r="C598" s="12"/>
+      <c r="C598" s="11"/>
     </row>
     <row r="599">
-      <c r="C599" s="12"/>
+      <c r="C599" s="11"/>
     </row>
     <row r="600">
-      <c r="C600" s="12"/>
+      <c r="C600" s="11"/>
     </row>
     <row r="601">
-      <c r="C601" s="12"/>
+      <c r="C601" s="11"/>
     </row>
     <row r="602">
-      <c r="C602" s="12"/>
+      <c r="C602" s="11"/>
     </row>
     <row r="603">
-      <c r="C603" s="12"/>
+      <c r="C603" s="11"/>
     </row>
     <row r="604">
-      <c r="C604" s="12"/>
+      <c r="C604" s="11"/>
     </row>
     <row r="605">
-      <c r="C605" s="12"/>
+      <c r="C605" s="11"/>
     </row>
     <row r="606">
-      <c r="C606" s="12"/>
+      <c r="C606" s="11"/>
     </row>
     <row r="607">
-      <c r="C607" s="12"/>
+      <c r="C607" s="11"/>
     </row>
     <row r="608">
-      <c r="C608" s="12"/>
+      <c r="C608" s="11"/>
     </row>
     <row r="609">
-      <c r="C609" s="12"/>
+      <c r="C609" s="11"/>
     </row>
     <row r="610">
-      <c r="C610" s="12"/>
+      <c r="C610" s="11"/>
     </row>
     <row r="611">
-      <c r="C611" s="12"/>
+      <c r="C611" s="11"/>
     </row>
     <row r="612">
-      <c r="C612" s="12"/>
+      <c r="C612" s="11"/>
     </row>
     <row r="613">
-      <c r="C613" s="12"/>
+      <c r="C613" s="11"/>
     </row>
     <row r="614">
-      <c r="C614" s="12"/>
+      <c r="C614" s="11"/>
     </row>
     <row r="615">
-      <c r="C615" s="12"/>
+      <c r="C615" s="11"/>
     </row>
     <row r="616">
-      <c r="C616" s="12"/>
+      <c r="C616" s="11"/>
     </row>
     <row r="617">
-      <c r="C617" s="12"/>
+      <c r="C617" s="11"/>
     </row>
     <row r="618">
-      <c r="C618" s="12"/>
+      <c r="C618" s="11"/>
     </row>
     <row r="619">
-      <c r="C619" s="12"/>
+      <c r="C619" s="11"/>
     </row>
     <row r="620">
-      <c r="C620" s="12"/>
+      <c r="C620" s="11"/>
     </row>
     <row r="621">
-      <c r="C621" s="12"/>
+      <c r="C621" s="11"/>
     </row>
     <row r="622">
-      <c r="C622" s="12"/>
+      <c r="C622" s="11"/>
     </row>
     <row r="623">
-      <c r="C623" s="12"/>
+      <c r="C623" s="11"/>
     </row>
     <row r="624">
-      <c r="C624" s="12"/>
+      <c r="C624" s="11"/>
     </row>
     <row r="625">
-      <c r="C625" s="12"/>
+      <c r="C625" s="11"/>
     </row>
     <row r="626">
-      <c r="C626" s="12"/>
+      <c r="C626" s="11"/>
     </row>
     <row r="627">
-      <c r="C627" s="12"/>
+      <c r="C627" s="11"/>
     </row>
     <row r="628">
-      <c r="C628" s="12"/>
+      <c r="C628" s="11"/>
     </row>
     <row r="629">
-      <c r="C629" s="12"/>
+      <c r="C629" s="11"/>
     </row>
     <row r="630">
-      <c r="C630" s="12"/>
+      <c r="C630" s="11"/>
     </row>
     <row r="631">
-      <c r="C631" s="12"/>
+      <c r="C631" s="11"/>
     </row>
     <row r="632">
-      <c r="C632" s="12"/>
+      <c r="C632" s="11"/>
     </row>
     <row r="633">
-      <c r="C633" s="12"/>
+      <c r="C633" s="11"/>
     </row>
     <row r="634">
-      <c r="C634" s="12"/>
+      <c r="C634" s="11"/>
     </row>
     <row r="635">
-      <c r="C635" s="12"/>
+      <c r="C635" s="11"/>
     </row>
     <row r="636">
-      <c r="C636" s="12"/>
+      <c r="C636" s="11"/>
     </row>
     <row r="637">
-      <c r="C637" s="12"/>
+      <c r="C637" s="11"/>
     </row>
     <row r="638">
-      <c r="C638" s="12"/>
+      <c r="C638" s="11"/>
     </row>
     <row r="639">
-      <c r="C639" s="12"/>
+      <c r="C639" s="11"/>
     </row>
     <row r="640">
-      <c r="C640" s="12"/>
+      <c r="C640" s="11"/>
     </row>
     <row r="641">
-      <c r="C641" s="12"/>
+      <c r="C641" s="11"/>
     </row>
     <row r="642">
-      <c r="C642" s="12"/>
+      <c r="C642" s="11"/>
     </row>
     <row r="643">
-      <c r="C643" s="12"/>
+      <c r="C643" s="11"/>
     </row>
     <row r="644">
-      <c r="C644" s="12"/>
+      <c r="C644" s="11"/>
     </row>
     <row r="645">
-      <c r="C645" s="12"/>
+      <c r="C645" s="11"/>
     </row>
     <row r="646">
-      <c r="C646" s="12"/>
+      <c r="C646" s="11"/>
     </row>
     <row r="647">
-      <c r="C647" s="12"/>
+      <c r="C647" s="11"/>
     </row>
     <row r="648">
-      <c r="C648" s="12"/>
+      <c r="C648" s="11"/>
     </row>
     <row r="649">
-      <c r="C649" s="12"/>
+      <c r="C649" s="11"/>
     </row>
     <row r="650">
-      <c r="C650" s="12"/>
+      <c r="C650" s="11"/>
     </row>
     <row r="651">
-      <c r="C651" s="12"/>
+      <c r="C651" s="11"/>
     </row>
     <row r="652">
-      <c r="C652" s="12"/>
+      <c r="C652" s="11"/>
     </row>
     <row r="653">
-      <c r="C653" s="12"/>
+      <c r="C653" s="11"/>
     </row>
     <row r="654">
-      <c r="C654" s="12"/>
+      <c r="C654" s="11"/>
     </row>
     <row r="655">
-      <c r="C655" s="12"/>
+      <c r="C655" s="11"/>
     </row>
     <row r="656">
-      <c r="C656" s="12"/>
+      <c r="C656" s="11"/>
     </row>
     <row r="657">
-      <c r="C657" s="12"/>
+      <c r="C657" s="11"/>
     </row>
     <row r="658">
-      <c r="C658" s="12"/>
+      <c r="C658" s="11"/>
     </row>
     <row r="659">
-      <c r="C659" s="12"/>
+      <c r="C659" s="11"/>
     </row>
     <row r="660">
-      <c r="C660" s="12"/>
+      <c r="C660" s="11"/>
     </row>
     <row r="661">
-      <c r="C661" s="12"/>
+      <c r="C661" s="11"/>
     </row>
     <row r="662">
-      <c r="C662" s="12"/>
+      <c r="C662" s="11"/>
     </row>
     <row r="663">
-      <c r="C663" s="12"/>
+      <c r="C663" s="11"/>
     </row>
     <row r="664">
-      <c r="C664" s="12"/>
+      <c r="C664" s="11"/>
     </row>
     <row r="665">
-      <c r="C665" s="12"/>
+      <c r="C665" s="11"/>
     </row>
     <row r="666">
-      <c r="C666" s="12"/>
+      <c r="C666" s="11"/>
     </row>
     <row r="667">
-      <c r="C667" s="12"/>
+      <c r="C667" s="11"/>
     </row>
     <row r="668">
-      <c r="C668" s="12"/>
+      <c r="C668" s="11"/>
     </row>
     <row r="669">
-      <c r="C669" s="12"/>
+      <c r="C669" s="11"/>
     </row>
     <row r="670">
-      <c r="C670" s="12"/>
+      <c r="C670" s="11"/>
     </row>
     <row r="671">
-      <c r="C671" s="12"/>
+      <c r="C671" s="11"/>
     </row>
     <row r="672">
-      <c r="C672" s="12"/>
+      <c r="C672" s="11"/>
     </row>
     <row r="673">
-      <c r="C673" s="12"/>
+      <c r="C673" s="11"/>
     </row>
     <row r="674">
-      <c r="C674" s="12"/>
+      <c r="C674" s="11"/>
     </row>
     <row r="675">
-      <c r="C675" s="12"/>
+      <c r="C675" s="11"/>
     </row>
     <row r="676">
-      <c r="C676" s="12"/>
+      <c r="C676" s="11"/>
     </row>
     <row r="677">
-      <c r="C677" s="12"/>
+      <c r="C677" s="11"/>
     </row>
     <row r="678">
-      <c r="C678" s="12"/>
+      <c r="C678" s="11"/>
     </row>
     <row r="679">
-      <c r="C679" s="12"/>
+      <c r="C679" s="11"/>
     </row>
     <row r="680">
-      <c r="C680" s="12"/>
+      <c r="C680" s="11"/>
     </row>
     <row r="681">
-      <c r="C681" s="12"/>
+      <c r="C681" s="11"/>
     </row>
     <row r="682">
-      <c r="C682" s="12"/>
+      <c r="C682" s="11"/>
     </row>
     <row r="683">
-      <c r="C683" s="12"/>
+      <c r="C683" s="11"/>
     </row>
     <row r="684">
-      <c r="C684" s="12"/>
+      <c r="C684" s="11"/>
     </row>
     <row r="685">
-      <c r="C685" s="12"/>
+      <c r="C685" s="11"/>
     </row>
     <row r="686">
-      <c r="C686" s="12"/>
+      <c r="C686" s="11"/>
     </row>
     <row r="687">
-      <c r="C687" s="12"/>
+      <c r="C687" s="11"/>
     </row>
     <row r="688">
-      <c r="C688" s="12"/>
+      <c r="C688" s="11"/>
     </row>
     <row r="689">
-      <c r="C689" s="12"/>
+      <c r="C689" s="11"/>
     </row>
     <row r="690">
-      <c r="C690" s="12"/>
+      <c r="C690" s="11"/>
     </row>
     <row r="691">
-      <c r="C691" s="12"/>
+      <c r="C691" s="11"/>
     </row>
     <row r="692">
-      <c r="C692" s="12"/>
+      <c r="C692" s="11"/>
     </row>
     <row r="693">
-      <c r="C693" s="12"/>
+      <c r="C693" s="11"/>
     </row>
     <row r="694">
-      <c r="C694" s="12"/>
+      <c r="C694" s="11"/>
     </row>
     <row r="695">
-      <c r="C695" s="12"/>
+      <c r="C695" s="11"/>
     </row>
     <row r="696">
-      <c r="C696" s="12"/>
+      <c r="C696" s="11"/>
     </row>
     <row r="697">
-      <c r="C697" s="12"/>
+      <c r="C697" s="11"/>
     </row>
     <row r="698">
-      <c r="C698" s="12"/>
+      <c r="C698" s="11"/>
     </row>
     <row r="699">
-      <c r="C699" s="12"/>
+      <c r="C699" s="11"/>
     </row>
     <row r="700">
-      <c r="C700" s="12"/>
+      <c r="C700" s="11"/>
     </row>
     <row r="701">
-      <c r="C701" s="12"/>
+      <c r="C701" s="11"/>
     </row>
     <row r="702">
-      <c r="C702" s="12"/>
+      <c r="C702" s="11"/>
     </row>
     <row r="703">
-      <c r="C703" s="12"/>
+      <c r="C703" s="11"/>
     </row>
     <row r="704">
-      <c r="C704" s="12"/>
+      <c r="C704" s="11"/>
     </row>
     <row r="705">
-      <c r="C705" s="12"/>
+      <c r="C705" s="11"/>
     </row>
     <row r="706">
-      <c r="C706" s="12"/>
+      <c r="C706" s="11"/>
     </row>
     <row r="707">
-      <c r="C707" s="12"/>
+      <c r="C707" s="11"/>
     </row>
     <row r="708">
-      <c r="C708" s="12"/>
+      <c r="C708" s="11"/>
     </row>
     <row r="709">
-      <c r="C709" s="12"/>
+      <c r="C709" s="11"/>
     </row>
     <row r="710">
-      <c r="C710" s="12"/>
+      <c r="C710" s="11"/>
     </row>
     <row r="711">
-      <c r="C711" s="12"/>
+      <c r="C711" s="11"/>
     </row>
     <row r="712">
-      <c r="C712" s="12"/>
+      <c r="C712" s="11"/>
     </row>
     <row r="713">
-      <c r="C713" s="12"/>
+      <c r="C713" s="11"/>
     </row>
     <row r="714">
-      <c r="C714" s="12"/>
+      <c r="C714" s="11"/>
     </row>
     <row r="715">
-      <c r="C715" s="12"/>
+      <c r="C715" s="11"/>
     </row>
     <row r="716">
-      <c r="C716" s="12"/>
+      <c r="C716" s="11"/>
     </row>
     <row r="717">
-      <c r="C717" s="12"/>
+      <c r="C717" s="11"/>
     </row>
     <row r="718">
-      <c r="C718" s="12"/>
+      <c r="C718" s="11"/>
     </row>
     <row r="719">
-      <c r="C719" s="12"/>
+      <c r="C719" s="11"/>
     </row>
     <row r="720">
-      <c r="C720" s="12"/>
+      <c r="C720" s="11"/>
     </row>
     <row r="721">
-      <c r="C721" s="12"/>
+      <c r="C721" s="11"/>
     </row>
     <row r="722">
-      <c r="C722" s="12"/>
+      <c r="C722" s="11"/>
     </row>
     <row r="723">
-      <c r="C723" s="12"/>
+      <c r="C723" s="11"/>
     </row>
     <row r="724">
-      <c r="C724" s="12"/>
+      <c r="C724" s="11"/>
     </row>
     <row r="725">
-      <c r="C725" s="12"/>
+      <c r="C725" s="11"/>
     </row>
     <row r="726">
-      <c r="C726" s="12"/>
+      <c r="C726" s="11"/>
     </row>
     <row r="727">
-      <c r="C727" s="12"/>
+      <c r="C727" s="11"/>
     </row>
     <row r="728">
-      <c r="C728" s="12"/>
+      <c r="C728" s="11"/>
     </row>
     <row r="729">
-      <c r="C729" s="12"/>
+      <c r="C729" s="11"/>
     </row>
     <row r="730">
-      <c r="C730" s="12"/>
+      <c r="C730" s="11"/>
     </row>
     <row r="731">
-      <c r="C731" s="12"/>
+      <c r="C731" s="11"/>
     </row>
     <row r="732">
-      <c r="C732" s="12"/>
+      <c r="C732" s="11"/>
     </row>
     <row r="733">
-      <c r="C733" s="12"/>
+      <c r="C733" s="11"/>
     </row>
     <row r="734">
-      <c r="C734" s="12"/>
+      <c r="C734" s="11"/>
     </row>
     <row r="735">
-      <c r="C735" s="12"/>
+      <c r="C735" s="11"/>
     </row>
     <row r="736">
-      <c r="C736" s="12"/>
+      <c r="C736" s="11"/>
     </row>
     <row r="737">
-      <c r="C737" s="12"/>
+      <c r="C737" s="11"/>
     </row>
     <row r="738">
-      <c r="C738" s="12"/>
+      <c r="C738" s="11"/>
     </row>
     <row r="739">
-      <c r="C739" s="12"/>
+      <c r="C739" s="11"/>
     </row>
     <row r="740">
-      <c r="C740" s="12"/>
+      <c r="C740" s="11"/>
     </row>
     <row r="741">
-      <c r="C741" s="12"/>
+      <c r="C741" s="11"/>
     </row>
     <row r="742">
-      <c r="C742" s="12"/>
+      <c r="C742" s="11"/>
     </row>
     <row r="743">
-      <c r="C743" s="12"/>
+      <c r="C743" s="11"/>
     </row>
     <row r="744">
-      <c r="C744" s="12"/>
+      <c r="C744" s="11"/>
     </row>
     <row r="745">
-      <c r="C745" s="12"/>
+      <c r="C745" s="11"/>
     </row>
     <row r="746">
-      <c r="C746" s="12"/>
+      <c r="C746" s="11"/>
     </row>
     <row r="747">
-      <c r="C747" s="12"/>
+      <c r="C747" s="11"/>
     </row>
     <row r="748">
-      <c r="C748" s="12"/>
+      <c r="C748" s="11"/>
     </row>
     <row r="749">
-      <c r="C749" s="12"/>
+      <c r="C749" s="11"/>
     </row>
     <row r="750">
-      <c r="C750" s="12"/>
+      <c r="C750" s="11"/>
     </row>
     <row r="751">
-      <c r="C751" s="12"/>
+      <c r="C751" s="11"/>
     </row>
     <row r="752">
-      <c r="C752" s="12"/>
+      <c r="C752" s="11"/>
     </row>
     <row r="753">
-      <c r="C753" s="12"/>
+      <c r="C753" s="11"/>
     </row>
     <row r="754">
-      <c r="C754" s="12"/>
+      <c r="C754" s="11"/>
     </row>
     <row r="755">
-      <c r="C755" s="12"/>
+      <c r="C755" s="11"/>
     </row>
     <row r="756">
-      <c r="C756" s="12"/>
+      <c r="C756" s="11"/>
     </row>
     <row r="757">
-      <c r="C757" s="12"/>
+      <c r="C757" s="11"/>
     </row>
     <row r="758">
-      <c r="C758" s="12"/>
+      <c r="C758" s="11"/>
     </row>
     <row r="759">
-      <c r="C759" s="12"/>
+      <c r="C759" s="11"/>
     </row>
     <row r="760">
-      <c r="C760" s="12"/>
+      <c r="C760" s="11"/>
     </row>
     <row r="761">
-      <c r="C761" s="12"/>
+      <c r="C761" s="11"/>
     </row>
     <row r="762">
-      <c r="C762" s="12"/>
+      <c r="C762" s="11"/>
     </row>
     <row r="763">
-      <c r="C763" s="12"/>
+      <c r="C763" s="11"/>
     </row>
     <row r="764">
-      <c r="C764" s="12"/>
+      <c r="C764" s="11"/>
     </row>
     <row r="765">
-      <c r="C765" s="12"/>
+      <c r="C765" s="11"/>
     </row>
     <row r="766">
-      <c r="C766" s="12"/>
+      <c r="C766" s="11"/>
     </row>
     <row r="767">
-      <c r="C767" s="12"/>
+      <c r="C767" s="11"/>
     </row>
     <row r="768">
-      <c r="C768" s="12"/>
+      <c r="C768" s="11"/>
     </row>
     <row r="769">
-      <c r="C769" s="12"/>
+      <c r="C769" s="11"/>
     </row>
     <row r="770">
-      <c r="C770" s="12"/>
+      <c r="C770" s="11"/>
     </row>
     <row r="771">
-      <c r="C771" s="12"/>
+      <c r="C771" s="11"/>
     </row>
     <row r="772">
-      <c r="C772" s="12"/>
+      <c r="C772" s="11"/>
     </row>
     <row r="773">
-      <c r="C773" s="12"/>
+      <c r="C773" s="11"/>
     </row>
     <row r="774">
-      <c r="C774" s="12"/>
+      <c r="C774" s="11"/>
     </row>
     <row r="775">
-      <c r="C775" s="12"/>
+      <c r="C775" s="11"/>
     </row>
     <row r="776">
-      <c r="C776" s="12"/>
+      <c r="C776" s="11"/>
     </row>
     <row r="777">
-      <c r="C777" s="12"/>
+      <c r="C777" s="11"/>
     </row>
     <row r="778">
-      <c r="C778" s="12"/>
+      <c r="C778" s="11"/>
     </row>
     <row r="779">
-      <c r="C779" s="12"/>
+      <c r="C779" s="11"/>
     </row>
     <row r="780">
-      <c r="C780" s="12"/>
+      <c r="C780" s="11"/>
     </row>
     <row r="781">
-      <c r="C781" s="12"/>
+      <c r="C781" s="11"/>
     </row>
     <row r="782">
-      <c r="C782" s="12"/>
+      <c r="C782" s="11"/>
     </row>
     <row r="783">
-      <c r="C783" s="12"/>
+      <c r="C783" s="11"/>
     </row>
     <row r="784">
-      <c r="C784" s="12"/>
+      <c r="C784" s="11"/>
     </row>
     <row r="785">
-      <c r="C785" s="12"/>
+      <c r="C785" s="11"/>
     </row>
     <row r="786">
-      <c r="C786" s="12"/>
+      <c r="C786" s="11"/>
     </row>
     <row r="787">
-      <c r="C787" s="12"/>
+      <c r="C787" s="11"/>
     </row>
     <row r="788">
-      <c r="C788" s="12"/>
+      <c r="C788" s="11"/>
     </row>
     <row r="789">
-      <c r="C789" s="12"/>
+      <c r="C789" s="11"/>
     </row>
     <row r="790">
-      <c r="C790" s="12"/>
+      <c r="C790" s="11"/>
     </row>
     <row r="791">
-      <c r="C791" s="12"/>
+      <c r="C791" s="11"/>
     </row>
     <row r="792">
-      <c r="C792" s="12"/>
+      <c r="C792" s="11"/>
     </row>
     <row r="793">
-      <c r="C793" s="12"/>
+      <c r="C793" s="11"/>
     </row>
     <row r="794">
-      <c r="C794" s="12"/>
+      <c r="C794" s="11"/>
     </row>
     <row r="795">
-      <c r="C795" s="12"/>
+      <c r="C795" s="11"/>
     </row>
     <row r="796">
-      <c r="C796" s="12"/>
+      <c r="C796" s="11"/>
     </row>
     <row r="797">
-      <c r="C797" s="12"/>
+      <c r="C797" s="11"/>
     </row>
     <row r="798">
-      <c r="C798" s="12"/>
+      <c r="C798" s="11"/>
     </row>
     <row r="799">
-      <c r="C799" s="12"/>
+      <c r="C799" s="11"/>
     </row>
     <row r="800">
-      <c r="C800" s="12"/>
+      <c r="C800" s="11"/>
     </row>
     <row r="801">
-      <c r="C801" s="12"/>
+      <c r="C801" s="11"/>
     </row>
     <row r="802">
-      <c r="C802" s="12"/>
+      <c r="C802" s="11"/>
     </row>
     <row r="803">
-      <c r="C803" s="12"/>
+      <c r="C803" s="11"/>
     </row>
     <row r="804">
-      <c r="C804" s="12"/>
+      <c r="C804" s="11"/>
     </row>
     <row r="805">
-      <c r="C805" s="12"/>
+      <c r="C805" s="11"/>
     </row>
     <row r="806">
-      <c r="C806" s="12"/>
+      <c r="C806" s="11"/>
     </row>
     <row r="807">
-      <c r="C807" s="12"/>
+      <c r="C807" s="11"/>
     </row>
     <row r="808">
-      <c r="C808" s="12"/>
+      <c r="C808" s="11"/>
     </row>
     <row r="809">
-      <c r="C809" s="12"/>
+      <c r="C809" s="11"/>
     </row>
     <row r="810">
-      <c r="C810" s="12"/>
+      <c r="C810" s="11"/>
     </row>
     <row r="811">
-      <c r="C811" s="12"/>
+      <c r="C811" s="11"/>
     </row>
     <row r="812">
-      <c r="C812" s="12"/>
+      <c r="C812" s="11"/>
     </row>
     <row r="813">
-      <c r="C813" s="12"/>
+      <c r="C813" s="11"/>
     </row>
     <row r="814">
-      <c r="C814" s="12"/>
+      <c r="C814" s="11"/>
     </row>
     <row r="815">
-      <c r="C815" s="12"/>
+      <c r="C815" s="11"/>
     </row>
     <row r="816">
-      <c r="C816" s="12"/>
+      <c r="C816" s="11"/>
     </row>
     <row r="817">
-      <c r="C817" s="12"/>
+      <c r="C817" s="11"/>
     </row>
     <row r="818">
-      <c r="C818" s="12"/>
+      <c r="C818" s="11"/>
     </row>
     <row r="819">
-      <c r="C819" s="12"/>
+      <c r="C819" s="11"/>
     </row>
     <row r="820">
-      <c r="C820" s="12"/>
+      <c r="C820" s="11"/>
     </row>
     <row r="821">
-      <c r="C821" s="12"/>
+      <c r="C821" s="11"/>
     </row>
     <row r="822">
-      <c r="C822" s="12"/>
+      <c r="C822" s="11"/>
     </row>
     <row r="823">
-      <c r="C823" s="12"/>
+      <c r="C823" s="11"/>
     </row>
     <row r="824">
-      <c r="C824" s="12"/>
+      <c r="C824" s="11"/>
     </row>
     <row r="825">
-      <c r="C825" s="12"/>
+      <c r="C825" s="11"/>
     </row>
     <row r="826">
-      <c r="C826" s="12"/>
+      <c r="C826" s="11"/>
     </row>
     <row r="827">
-      <c r="C827" s="12"/>
+      <c r="C827" s="11"/>
     </row>
     <row r="828">
-      <c r="C828" s="12"/>
+      <c r="C828" s="11"/>
     </row>
     <row r="829">
-      <c r="C829" s="12"/>
+      <c r="C829" s="11"/>
     </row>
     <row r="830">
-      <c r="C830" s="12"/>
+      <c r="C830" s="11"/>
     </row>
     <row r="831">
-      <c r="C831" s="12"/>
+      <c r="C831" s="11"/>
     </row>
     <row r="832">
-      <c r="C832" s="12"/>
+      <c r="C832" s="11"/>
     </row>
     <row r="833">
-      <c r="C833" s="12"/>
+      <c r="C833" s="11"/>
     </row>
     <row r="834">
-      <c r="C834" s="12"/>
+      <c r="C834" s="11"/>
     </row>
     <row r="835">
-      <c r="C835" s="12"/>
+      <c r="C835" s="11"/>
     </row>
     <row r="836">
-      <c r="C836" s="12"/>
+      <c r="C836" s="11"/>
     </row>
     <row r="837">
-      <c r="C837" s="12"/>
+      <c r="C837" s="11"/>
     </row>
     <row r="838">
-      <c r="C838" s="12"/>
+      <c r="C838" s="11"/>
     </row>
     <row r="839">
-      <c r="C839" s="12"/>
+      <c r="C839" s="11"/>
     </row>
     <row r="840">
-      <c r="C840" s="12"/>
+      <c r="C840" s="11"/>
     </row>
     <row r="841">
-      <c r="C841" s="12"/>
+      <c r="C841" s="11"/>
     </row>
     <row r="842">
-      <c r="C842" s="12"/>
+      <c r="C842" s="11"/>
     </row>
     <row r="843">
-      <c r="C843" s="12"/>
+      <c r="C843" s="11"/>
     </row>
     <row r="844">
-      <c r="C844" s="12"/>
+      <c r="C844" s="11"/>
     </row>
     <row r="845">
-      <c r="C845" s="12"/>
+      <c r="C845" s="11"/>
     </row>
     <row r="846">
-      <c r="C846" s="12"/>
+      <c r="C846" s="11"/>
     </row>
     <row r="847">
-      <c r="C847" s="12"/>
+      <c r="C847" s="11"/>
     </row>
     <row r="848">
-      <c r="C848" s="12"/>
+      <c r="C848" s="11"/>
     </row>
     <row r="849">
-      <c r="C849" s="12"/>
+      <c r="C849" s="11"/>
     </row>
     <row r="850">
-      <c r="C850" s="12"/>
+      <c r="C850" s="11"/>
     </row>
     <row r="851">
-      <c r="C851" s="12"/>
+      <c r="C851" s="11"/>
     </row>
     <row r="852">
-      <c r="C852" s="12"/>
+      <c r="C852" s="11"/>
     </row>
     <row r="853">
-      <c r="C853" s="12"/>
+      <c r="C853" s="11"/>
     </row>
     <row r="854">
-      <c r="C854" s="12"/>
+      <c r="C854" s="11"/>
     </row>
     <row r="855">
-      <c r="C855" s="12"/>
+      <c r="C855" s="11"/>
     </row>
     <row r="856">
-      <c r="C856" s="12"/>
+      <c r="C856" s="11"/>
     </row>
     <row r="857">
-      <c r="C857" s="12"/>
+      <c r="C857" s="11"/>
     </row>
     <row r="858">
-      <c r="C858" s="12"/>
+      <c r="C858" s="11"/>
     </row>
     <row r="859">
-      <c r="C859" s="12"/>
+      <c r="C859" s="11"/>
     </row>
     <row r="860">
-      <c r="C860" s="12"/>
+      <c r="C860" s="11"/>
     </row>
     <row r="861">
-      <c r="C861" s="12"/>
+      <c r="C861" s="11"/>
     </row>
     <row r="862">
-      <c r="C862" s="12"/>
+      <c r="C862" s="11"/>
     </row>
     <row r="863">
-      <c r="C863" s="12"/>
+      <c r="C863" s="11"/>
     </row>
     <row r="864">
-      <c r="C864" s="12"/>
+      <c r="C864" s="11"/>
     </row>
     <row r="865">
-      <c r="C865" s="12"/>
+      <c r="C865" s="11"/>
     </row>
     <row r="866">
-      <c r="C866" s="12"/>
+      <c r="C866" s="11"/>
     </row>
     <row r="867">
-      <c r="C867" s="12"/>
+      <c r="C867" s="11"/>
     </row>
     <row r="868">
-      <c r="C868" s="12"/>
+      <c r="C868" s="11"/>
     </row>
     <row r="869">
-      <c r="C869" s="12"/>
+      <c r="C869" s="11"/>
     </row>
     <row r="870">
-      <c r="C870" s="12"/>
+      <c r="C870" s="11"/>
     </row>
     <row r="871">
-      <c r="C871" s="12"/>
+      <c r="C871" s="11"/>
     </row>
     <row r="872">
-      <c r="C872" s="12"/>
+      <c r="C872" s="11"/>
     </row>
     <row r="873">
-      <c r="C873" s="12"/>
+      <c r="C873" s="11"/>
     </row>
     <row r="874">
-      <c r="C874" s="12"/>
+      <c r="C874" s="11"/>
     </row>
     <row r="875">
-      <c r="C875" s="12"/>
+      <c r="C875" s="11"/>
     </row>
     <row r="876">
-      <c r="C876" s="12"/>
+      <c r="C876" s="11"/>
     </row>
     <row r="877">
-      <c r="C877" s="12"/>
+      <c r="C877" s="11"/>
     </row>
     <row r="878">
-      <c r="C878" s="12"/>
+      <c r="C878" s="11"/>
     </row>
     <row r="879">
-      <c r="C879" s="12"/>
+      <c r="C879" s="11"/>
     </row>
     <row r="880">
-      <c r="C880" s="12"/>
+      <c r="C880" s="11"/>
     </row>
     <row r="881">
-      <c r="C881" s="12"/>
+      <c r="C881" s="11"/>
     </row>
     <row r="882">
-      <c r="C882" s="12"/>
+      <c r="C882" s="11"/>
     </row>
     <row r="883">
-      <c r="C883" s="12"/>
+      <c r="C883" s="11"/>
     </row>
     <row r="884">
-      <c r="C884" s="12"/>
+      <c r="C884" s="11"/>
     </row>
     <row r="885">
-      <c r="C885" s="12"/>
+      <c r="C885" s="11"/>
     </row>
     <row r="886">
-      <c r="C886" s="12"/>
+      <c r="C886" s="11"/>
     </row>
     <row r="887">
-      <c r="C887" s="12"/>
+      <c r="C887" s="11"/>
     </row>
     <row r="888">
-      <c r="C888" s="12"/>
+      <c r="C888" s="11"/>
     </row>
     <row r="889">
-      <c r="C889" s="12"/>
+      <c r="C889" s="11"/>
     </row>
     <row r="890">
-      <c r="C890" s="12"/>
+      <c r="C890" s="11"/>
     </row>
     <row r="891">
-      <c r="C891" s="12"/>
+      <c r="C891" s="11"/>
     </row>
     <row r="892">
-      <c r="C892" s="12"/>
+      <c r="C892" s="11"/>
     </row>
     <row r="893">
-      <c r="C893" s="12"/>
+      <c r="C893" s="11"/>
     </row>
     <row r="894">
-      <c r="C894" s="12"/>
+      <c r="C894" s="11"/>
     </row>
     <row r="895">
-      <c r="C895" s="12"/>
+      <c r="C895" s="11"/>
     </row>
     <row r="896">
-      <c r="C896" s="12"/>
+      <c r="C896" s="11"/>
     </row>
     <row r="897">
-      <c r="C897" s="12"/>
+      <c r="C897" s="11"/>
     </row>
     <row r="898">
-      <c r="C898" s="12"/>
+      <c r="C898" s="11"/>
     </row>
     <row r="899">
-      <c r="C899" s="12"/>
+      <c r="C899" s="11"/>
     </row>
     <row r="900">
-      <c r="C900" s="12"/>
+      <c r="C900" s="11"/>
     </row>
     <row r="901">
-      <c r="C901" s="12"/>
+      <c r="C901" s="11"/>
     </row>
     <row r="902">
-      <c r="C902" s="12"/>
+      <c r="C902" s="11"/>
     </row>
     <row r="903">
-      <c r="C903" s="12"/>
+      <c r="C903" s="11"/>
     </row>
     <row r="904">
-      <c r="C904" s="12"/>
+      <c r="C904" s="11"/>
     </row>
     <row r="905">
-      <c r="C905" s="12"/>
+      <c r="C905" s="11"/>
     </row>
     <row r="906">
-      <c r="C906" s="12"/>
+      <c r="C906" s="11"/>
     </row>
     <row r="907">
-      <c r="C907" s="12"/>
+      <c r="C907" s="11"/>
     </row>
     <row r="908">
-      <c r="C908" s="12"/>
+      <c r="C908" s="11"/>
     </row>
     <row r="909">
-      <c r="C909" s="12"/>
+      <c r="C909" s="11"/>
     </row>
     <row r="910">
-      <c r="C910" s="12"/>
+      <c r="C910" s="11"/>
     </row>
     <row r="911">
-      <c r="C911" s="12"/>
+      <c r="C911" s="11"/>
     </row>
     <row r="912">
-      <c r="C912" s="12"/>
+      <c r="C912" s="11"/>
     </row>
     <row r="913">
-      <c r="C913" s="12"/>
+      <c r="C913" s="11"/>
     </row>
     <row r="914">
-      <c r="C914" s="12"/>
+      <c r="C914" s="11"/>
     </row>
     <row r="915">
-      <c r="C915" s="12"/>
+      <c r="C915" s="11"/>
     </row>
     <row r="916">
-      <c r="C916" s="12"/>
+      <c r="C916" s="11"/>
     </row>
     <row r="917">
-      <c r="C917" s="12"/>
+      <c r="C917" s="11"/>
     </row>
     <row r="918">
-      <c r="C918" s="12"/>
+      <c r="C918" s="11"/>
     </row>
     <row r="919">
-      <c r="C919" s="12"/>
+      <c r="C919" s="11"/>
     </row>
     <row r="920">
-      <c r="C920" s="12"/>
+      <c r="C920" s="11"/>
     </row>
     <row r="921">
-      <c r="C921" s="12"/>
+      <c r="C921" s="11"/>
     </row>
     <row r="922">
-      <c r="C922" s="12"/>
+      <c r="C922" s="11"/>
     </row>
     <row r="923">
-      <c r="C923" s="12"/>
+      <c r="C923" s="11"/>
     </row>
     <row r="924">
-      <c r="C924" s="12"/>
+      <c r="C924" s="11"/>
     </row>
     <row r="925">
-      <c r="C925" s="12"/>
+      <c r="C925" s="11"/>
     </row>
     <row r="926">
-      <c r="C926" s="12"/>
+      <c r="C926" s="11"/>
     </row>
     <row r="927">
-      <c r="C927" s="12"/>
+      <c r="C927" s="11"/>
     </row>
     <row r="928">
-      <c r="C928" s="12"/>
+      <c r="C928" s="11"/>
     </row>
     <row r="929">
-      <c r="C929" s="12"/>
+      <c r="C929" s="11"/>
     </row>
     <row r="930">
-      <c r="C930" s="12"/>
+      <c r="C930" s="11"/>
     </row>
     <row r="931">
-      <c r="C931" s="12"/>
+      <c r="C931" s="11"/>
     </row>
     <row r="932">
-      <c r="C932" s="12"/>
+      <c r="C932" s="11"/>
     </row>
     <row r="933">
-      <c r="C933" s="12"/>
+      <c r="C933" s="11"/>
     </row>
     <row r="934">
-      <c r="C934" s="12"/>
+      <c r="C934" s="11"/>
     </row>
     <row r="935">
-      <c r="C935" s="12"/>
+      <c r="C935" s="11"/>
     </row>
     <row r="936">
-      <c r="C936" s="12"/>
+      <c r="C936" s="11"/>
     </row>
     <row r="937">
-      <c r="C937" s="12"/>
+      <c r="C937" s="11"/>
     </row>
     <row r="938">
-      <c r="C938" s="12"/>
+      <c r="C938" s="11"/>
     </row>
     <row r="939">
-      <c r="C939" s="12"/>
+      <c r="C939" s="11"/>
     </row>
     <row r="940">
-      <c r="C940" s="12"/>
+      <c r="C940" s="11"/>
     </row>
     <row r="941">
-      <c r="C941" s="12"/>
+      <c r="C941" s="11"/>
     </row>
     <row r="942">
-      <c r="C942" s="12"/>
+      <c r="C942" s="11"/>
     </row>
     <row r="943">
-      <c r="C943" s="12"/>
+      <c r="C943" s="11"/>
     </row>
     <row r="944">
-      <c r="C944" s="12"/>
+      <c r="C944" s="11"/>
     </row>
     <row r="945">
-      <c r="C945" s="12"/>
+      <c r="C945" s="11"/>
     </row>
     <row r="946">
-      <c r="C946" s="12"/>
+      <c r="C946" s="11"/>
     </row>
     <row r="947">
-      <c r="C947" s="12"/>
+      <c r="C947" s="11"/>
     </row>
     <row r="948">
-      <c r="C948" s="12"/>
+      <c r="C948" s="11"/>
     </row>
     <row r="949">
-      <c r="C949" s="12"/>
+      <c r="C949" s="11"/>
     </row>
     <row r="950">
-      <c r="C950" s="12"/>
+      <c r="C950" s="11"/>
     </row>
     <row r="951">
-      <c r="C951" s="12"/>
+      <c r="C951" s="11"/>
     </row>
     <row r="952">
-      <c r="C952" s="12"/>
+      <c r="C952" s="11"/>
     </row>
     <row r="953">
-      <c r="C953" s="12"/>
+      <c r="C953" s="11"/>
     </row>
     <row r="954">
-      <c r="C954" s="12"/>
+      <c r="C954" s="11"/>
     </row>
     <row r="955">
-      <c r="C955" s="12"/>
+      <c r="C955" s="11"/>
     </row>
     <row r="956">
-      <c r="C956" s="12"/>
+      <c r="C956" s="11"/>
     </row>
     <row r="957">
-      <c r="C957" s="12"/>
+      <c r="C957" s="11"/>
     </row>
     <row r="958">
-      <c r="C958" s="12"/>
+      <c r="C958" s="11"/>
     </row>
     <row r="959">
-      <c r="C959" s="12"/>
+      <c r="C959" s="11"/>
     </row>
     <row r="960">
-      <c r="C960" s="12"/>
+      <c r="C960" s="11"/>
     </row>
     <row r="961">
-      <c r="C961" s="12"/>
+      <c r="C961" s="11"/>
     </row>
     <row r="962">
-      <c r="C962" s="12"/>
+      <c r="C962" s="11"/>
     </row>
     <row r="963">
-      <c r="C963" s="12"/>
+      <c r="C963" s="11"/>
     </row>
     <row r="964">
-      <c r="C964" s="12"/>
+      <c r="C964" s="11"/>
     </row>
     <row r="965">
-      <c r="C965" s="12"/>
+      <c r="C965" s="11"/>
     </row>
     <row r="966">
-      <c r="C966" s="12"/>
+      <c r="C966" s="11"/>
     </row>
     <row r="967">
-      <c r="C967" s="12"/>
+      <c r="C967" s="11"/>
     </row>
     <row r="968">
-      <c r="C968" s="12"/>
+      <c r="C968" s="11"/>
     </row>
     <row r="969">
-      <c r="C969" s="12"/>
+      <c r="C969" s="11"/>
     </row>
     <row r="970">
-      <c r="C970" s="12"/>
+      <c r="C970" s="11"/>
     </row>
     <row r="971">
-      <c r="C971" s="12"/>
+      <c r="C971" s="11"/>
     </row>
     <row r="972">
-      <c r="C972" s="12"/>
+      <c r="C972" s="11"/>
     </row>
     <row r="973">
-      <c r="C973" s="12"/>
+      <c r="C973" s="11"/>
     </row>
     <row r="974">
-      <c r="C974" s="12"/>
+      <c r="C974" s="11"/>
     </row>
     <row r="975">
-      <c r="C975" s="12"/>
+      <c r="C975" s="11"/>
     </row>
     <row r="976">
-      <c r="C976" s="12"/>
+      <c r="C976" s="11"/>
     </row>
     <row r="977">
-      <c r="C977" s="12"/>
+      <c r="C977" s="11"/>
     </row>
     <row r="978">
-      <c r="C978" s="12"/>
+      <c r="C978" s="11"/>
     </row>
     <row r="979">
-      <c r="C979" s="12"/>
+      <c r="C979" s="11"/>
     </row>
     <row r="980">
-      <c r="C980" s="12"/>
+      <c r="C980" s="11"/>
     </row>
     <row r="981">
-      <c r="C981" s="12"/>
+      <c r="C981" s="11"/>
     </row>
     <row r="982">
-      <c r="C982" s="12"/>
+      <c r="C982" s="11"/>
     </row>
     <row r="983">
-      <c r="C983" s="12"/>
+      <c r="C983" s="11"/>
     </row>
     <row r="984">
-      <c r="C984" s="12"/>
+      <c r="C984" s="11"/>
     </row>
     <row r="985">
-      <c r="C985" s="12"/>
+      <c r="C985" s="11"/>
     </row>
     <row r="986">
-      <c r="C986" s="12"/>
+      <c r="C986" s="11"/>
     </row>
     <row r="987">
-      <c r="C987" s="12"/>
+      <c r="C987" s="11"/>
     </row>
     <row r="988">
-      <c r="C988" s="12"/>
+      <c r="C988" s="11"/>
     </row>
     <row r="989">
-      <c r="C989" s="12"/>
+      <c r="C989" s="11"/>
     </row>
     <row r="990">
-      <c r="C990" s="12"/>
+      <c r="C990" s="11"/>
     </row>
     <row r="991">
-      <c r="C991" s="12"/>
+      <c r="C991" s="11"/>
     </row>
     <row r="992">
-      <c r="C992" s="12"/>
+      <c r="C992" s="11"/>
     </row>
     <row r="993">
-      <c r="C993" s="12"/>
+      <c r="C993" s="11"/>
     </row>
     <row r="994">
-      <c r="C994" s="12"/>
+      <c r="C994" s="11"/>
     </row>
     <row r="995">
-      <c r="C995" s="12"/>
+      <c r="C995" s="11"/>
     </row>
     <row r="996">
-      <c r="C996" s="12"/>
+      <c r="C996" s="11"/>
     </row>
     <row r="997">
-      <c r="C997" s="12"/>
+      <c r="C997" s="11"/>
     </row>
     <row r="998">
-      <c r="C998" s="12"/>
+      <c r="C998" s="11"/>
     </row>
     <row r="999">
-      <c r="C999" s="12"/>
+      <c r="C999" s="11"/>
     </row>
     <row r="1000">
-      <c r="C1000" s="12"/>
+      <c r="C1000" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -8768,8 +8749,8 @@
     <hyperlink r:id="rId3" ref="G2"/>
     <hyperlink r:id="rId4" ref="F4"/>
     <hyperlink r:id="rId5" ref="F6"/>
-    <hyperlink r:id="rId6" ref="F8"/>
-    <hyperlink r:id="rId7" ref="C10"/>
+    <hyperlink r:id="rId6" ref="F9"/>
+    <hyperlink r:id="rId7" ref="F10"/>
     <hyperlink r:id="rId8" ref="F27"/>
     <hyperlink r:id="rId9" ref="F28"/>
     <hyperlink r:id="rId10" ref="F29"/>

</xml_diff>